<commit_message>
update period january 2025
</commit_message>
<xml_diff>
--- a/13_Period_20_Dec_2024_sd_19_Jan_2025/Timesheet Danamon_Bayu Bagus Bagaswara_January.xlsx
+++ b/13_Period_20_Dec_2024_sd_19_Jan_2025/Timesheet Danamon_Bayu Bagus Bagaswara_January.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bankdanamonindonesia-my.sharepoint.com/personal/v00028684_danamon_co_id/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayub\Projects Bayu\TIMESHEET DANAMON BAYU\13_Period_20_Dec_2024_sd_19_Jan_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{E58959C0-AE5B-42AE-AFC7-9E35B7F9C350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF49C831-827C-43E0-84A7-289988E4802F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD80C24C-653D-4C3A-8B9D-22F5F9620409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="1" activeTab="1" xr2:uid="{287076C2-500C-4AE4-B01E-3C74A6B599A0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{287076C2-500C-4AE4-B01E-3C74A6B599A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Timesheet_Template (OLD)" sheetId="28" state="hidden" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Timesheet_Template (OLD)'!$A$1:$AL$49</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="184">
   <si>
     <t>Timesheet Period</t>
   </si>
@@ -274,12 +274,6 @@
   </si>
   <si>
     <t>* = optional</t>
-  </si>
-  <si>
-    <t>Britney</t>
-  </si>
-  <si>
-    <t>Spears</t>
   </si>
   <si>
     <t xml:space="preserve">TIMESHEET GUIDELINE </t>
@@ -703,6 +697,71 @@
       <t xml:space="preserve">
 Harry Potter</t>
     </r>
+  </si>
+  <si>
+    <t>Bayu Bagus Bagaswara</t>
+  </si>
+  <si>
+    <t>IT Java Developer</t>
+  </si>
+  <si>
+    <t>Edy Yanto</t>
+  </si>
+  <si>
+    <t>Dody Arya</t>
+  </si>
+  <si>
+    <t>PO.67515</t>
+  </si>
+  <si>
+    <t>Bank Danamon Falatehan</t>
+  </si>
+  <si>
+    <t>Daily IT TFC</t>
+  </si>
+  <si>
+    <t>please drop your signature here
+Dody Arya</t>
+  </si>
+  <si>
+    <t>Added the TestDROIncomeController class as a data connection and test for Income query.</t>
+  </si>
+  <si>
+    <t>Added the TestDROLBABKController class as a data connection and test for LBABK query.</t>
+  </si>
+  <si>
+    <t>Added the TestDROLKPBUController class as a data connection and test for LKPBU query.</t>
+  </si>
+  <si>
+    <t>Create a new API with the /get-dro endpoint in LBABKController and connect it to the LBABKDROService service.</t>
+  </si>
+  <si>
+    <t>Create a new API with the /get-dro endpoint in LKPBUController and connect it to the LKPBUDROService service.</t>
+  </si>
+  <si>
+    <t>Create a new API with the /get-dro endpoint in LKPBUIncomeController and connect it to the LKPBUIncomeDROService service.</t>
+  </si>
+  <si>
+    <t>Create a logic layer LBABKDROService. Create a loadQuery method for query_get_lbabk.sql. Create a connection to the hiport database and map the query result data to variable LBABKDataSource objects.</t>
+  </si>
+  <si>
+    <t>Create a logic layer LKPBUDROService. Create a loadQuery method for query_get_lkpbu.sql. Create a connection to the hiport database and map the query result data to variable LKPBUDataSource objects.</t>
+  </si>
+  <si>
+    <t>Create a logic layer LKPBUIncomeDROService. Create a loadQuery method for query_get_income.sql. Create a connection to the hiport database and map the query result data to variable LKPBUIncome objects.</t>
+  </si>
+  <si>
+    <t>Changed the encapsulation of some methods in the CsvDataMapper utility so that they can be accessed from other classes. Added methods for data parsing such as, checkAndConvertSheetUnitLKPBU, parseSettleDateLBABK, parseSettleDateIncome, getKodeEfekLKPBU, parseToBigDecimalLKPBU, parseToBigDecimalLBABK, parseToBigDecimalIncome.</t>
+  </si>
+  <si>
+    <t>Monitoring generate LKPBU</t>
+  </si>
+  <si>
+    <t>CRF-5094</t>
+  </si>
+  <si>
+    <t>19-Jan-2025
+Bayu Bagus Bagaswara</t>
   </si>
 </sst>
 </file>
@@ -1505,7 +1564,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="206">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1908,6 +1967,12 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2037,6 +2102,15 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2090,6 +2164,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2118,14 +2195,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2728,12 +2805,12 @@
       </c>
       <c r="L5" s="78"/>
       <c r="M5" s="78"/>
-      <c r="N5" s="142" t="s">
+      <c r="N5" s="144" t="s">
         <v>11</v>
       </c>
-      <c r="O5" s="142"/>
-      <c r="P5" s="142"/>
-      <c r="Q5" s="142"/>
+      <c r="O5" s="144"/>
+      <c r="P5" s="144"/>
+      <c r="Q5" s="144"/>
     </row>
     <row r="6" spans="1:35" ht="17" x14ac:dyDescent="0.4">
       <c r="A6" s="74" t="s">
@@ -2758,12 +2835,12 @@
       </c>
       <c r="L6" s="87"/>
       <c r="M6" s="76"/>
-      <c r="N6" s="141" t="s">
+      <c r="N6" s="143" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="141"/>
-      <c r="P6" s="141"/>
-      <c r="Q6" s="141"/>
+      <c r="O6" s="143"/>
+      <c r="P6" s="143"/>
+      <c r="Q6" s="143"/>
       <c r="W6"/>
     </row>
     <row r="7" spans="1:35" s="42" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -2786,13 +2863,13 @@
       <c r="Q7" s="76"/>
     </row>
     <row r="9" spans="1:35" ht="17" x14ac:dyDescent="0.35">
-      <c r="A9" s="175" t="s">
+      <c r="A9" s="177" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="139" t="s">
+      <c r="B9" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="175" t="s">
+      <c r="C9" s="177" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="50" t="str">
@@ -2915,7 +2992,7 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="AH9" s="139" t="s">
+      <c r="AH9" s="141" t="s">
         <v>23</v>
       </c>
       <c r="AI9" s="90" t="s">
@@ -2923,9 +3000,9 @@
       </c>
     </row>
     <row r="10" spans="1:35" ht="17" x14ac:dyDescent="0.35">
-      <c r="A10" s="175"/>
-      <c r="B10" s="139"/>
-      <c r="C10" s="175"/>
+      <c r="A10" s="177"/>
+      <c r="B10" s="141"/>
+      <c r="C10" s="177"/>
       <c r="D10" s="51" cm="1">
         <f t="array" ref="D10:AG10">IFERROR(IF(OR((B3-B2+1)&gt;31,B2="",B3=""),"",_xlfn.SEQUENCE(,B3-B2+1,B2)),"")</f>
         <v>45536</v>
@@ -3017,7 +3094,7 @@
       <c r="AG10" s="51">
         <v>45565</v>
       </c>
-      <c r="AH10" s="139"/>
+      <c r="AH10" s="141"/>
       <c r="AI10" s="90"/>
     </row>
     <row r="11" spans="1:35" ht="17" x14ac:dyDescent="0.4">
@@ -3629,11 +3706,11 @@
       <c r="AI21" s="73"/>
     </row>
     <row r="22" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A22" s="176" t="s">
+      <c r="A22" s="178" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="177"/>
-      <c r="C22" s="178"/>
+      <c r="B22" s="179"/>
+      <c r="C22" s="180"/>
       <c r="D22" s="57"/>
       <c r="E22" s="57">
         <v>8</v>
@@ -3677,11 +3754,11 @@
       <c r="AI22" s="73"/>
     </row>
     <row r="23" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A23" s="176" t="s">
+      <c r="A23" s="178" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="177"/>
-      <c r="C23" s="178"/>
+      <c r="B23" s="179"/>
+      <c r="C23" s="180"/>
       <c r="D23" s="57"/>
       <c r="E23" s="57"/>
       <c r="F23" s="57">
@@ -3721,11 +3798,11 @@
       <c r="AI23" s="73"/>
     </row>
     <row r="24" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A24" s="179" t="s">
+      <c r="A24" s="181" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="180"/>
-      <c r="C24" s="181"/>
+      <c r="B24" s="182"/>
+      <c r="C24" s="183"/>
       <c r="D24" s="57"/>
       <c r="E24" s="57"/>
       <c r="F24" s="57"/>
@@ -3765,11 +3842,11 @@
       <c r="AI24" s="73"/>
     </row>
     <row r="25" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A25" s="176" t="s">
+      <c r="A25" s="178" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="177"/>
-      <c r="C25" s="178"/>
+      <c r="B25" s="179"/>
+      <c r="C25" s="180"/>
       <c r="D25" s="57"/>
       <c r="E25" s="57">
         <f t="shared" ref="E25:AB25" si="1">SUM(E11:E20)</f>
@@ -3900,145 +3977,145 @@
         <v>42</v>
       </c>
       <c r="D27" s="4"/>
-      <c r="E27" s="143"/>
-      <c r="F27" s="143"/>
-      <c r="G27" s="143"/>
-      <c r="H27" s="143"/>
-      <c r="I27" s="143"/>
-      <c r="J27" s="143"/>
-      <c r="S27" s="162" t="s">
+      <c r="E27" s="145"/>
+      <c r="F27" s="145"/>
+      <c r="G27" s="145"/>
+      <c r="H27" s="145"/>
+      <c r="I27" s="145"/>
+      <c r="J27" s="145"/>
+      <c r="S27" s="164" t="s">
         <v>43</v>
       </c>
-      <c r="T27" s="163"/>
-      <c r="U27" s="163"/>
-      <c r="V27" s="163"/>
-      <c r="W27" s="163"/>
-      <c r="X27" s="163"/>
-      <c r="Y27" s="163"/>
-      <c r="Z27" s="163"/>
-      <c r="AA27" s="164"/>
-      <c r="AC27" s="170" t="s">
+      <c r="T27" s="165"/>
+      <c r="U27" s="165"/>
+      <c r="V27" s="165"/>
+      <c r="W27" s="165"/>
+      <c r="X27" s="165"/>
+      <c r="Y27" s="165"/>
+      <c r="Z27" s="165"/>
+      <c r="AA27" s="166"/>
+      <c r="AC27" s="172" t="s">
         <v>44</v>
       </c>
-      <c r="AD27" s="171"/>
-      <c r="AE27" s="171"/>
-      <c r="AF27" s="171"/>
-      <c r="AG27" s="171"/>
-      <c r="AH27" s="171"/>
-      <c r="AI27" s="171"/>
-      <c r="AJ27" s="172"/>
+      <c r="AD27" s="173"/>
+      <c r="AE27" s="173"/>
+      <c r="AF27" s="173"/>
+      <c r="AG27" s="173"/>
+      <c r="AH27" s="173"/>
+      <c r="AI27" s="173"/>
+      <c r="AJ27" s="174"/>
     </row>
     <row r="28" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="69"/>
       <c r="B28" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="143"/>
-      <c r="F28" s="143"/>
-      <c r="G28" s="143"/>
-      <c r="H28" s="143"/>
-      <c r="I28" s="143"/>
-      <c r="J28" s="143"/>
-      <c r="S28" s="153" t="s">
+      <c r="E28" s="145"/>
+      <c r="F28" s="145"/>
+      <c r="G28" s="145"/>
+      <c r="H28" s="145"/>
+      <c r="I28" s="145"/>
+      <c r="J28" s="145"/>
+      <c r="S28" s="155" t="s">
         <v>46</v>
       </c>
-      <c r="T28" s="154"/>
-      <c r="U28" s="144" t="s">
+      <c r="T28" s="156"/>
+      <c r="U28" s="146" t="s">
         <v>47</v>
       </c>
-      <c r="V28" s="145"/>
-      <c r="W28" s="145"/>
-      <c r="X28" s="145"/>
-      <c r="Y28" s="145"/>
-      <c r="Z28" s="145"/>
-      <c r="AA28" s="146"/>
-      <c r="AC28" s="159" t="s">
+      <c r="V28" s="147"/>
+      <c r="W28" s="147"/>
+      <c r="X28" s="147"/>
+      <c r="Y28" s="147"/>
+      <c r="Z28" s="147"/>
+      <c r="AA28" s="148"/>
+      <c r="AC28" s="161" t="s">
         <v>48</v>
       </c>
-      <c r="AD28" s="145"/>
-      <c r="AE28" s="145"/>
-      <c r="AF28" s="145"/>
-      <c r="AG28" s="145"/>
-      <c r="AH28" s="145"/>
-      <c r="AI28" s="145"/>
-      <c r="AJ28" s="146"/>
+      <c r="AD28" s="147"/>
+      <c r="AE28" s="147"/>
+      <c r="AF28" s="147"/>
+      <c r="AG28" s="147"/>
+      <c r="AH28" s="147"/>
+      <c r="AI28" s="147"/>
+      <c r="AJ28" s="148"/>
     </row>
     <row r="29" spans="1:36" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="70"/>
       <c r="B29" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="E29" s="143"/>
-      <c r="F29" s="143"/>
-      <c r="G29" s="143"/>
-      <c r="H29" s="143"/>
-      <c r="I29" s="143"/>
-      <c r="J29" s="143"/>
-      <c r="S29" s="155"/>
-      <c r="T29" s="156"/>
-      <c r="U29" s="147"/>
-      <c r="V29" s="148"/>
-      <c r="W29" s="148"/>
-      <c r="X29" s="148"/>
-      <c r="Y29" s="148"/>
-      <c r="Z29" s="148"/>
-      <c r="AA29" s="149"/>
-      <c r="AC29" s="160"/>
-      <c r="AD29" s="148"/>
-      <c r="AE29" s="148"/>
-      <c r="AF29" s="148"/>
-      <c r="AG29" s="148"/>
-      <c r="AH29" s="148"/>
-      <c r="AI29" s="148"/>
-      <c r="AJ29" s="149"/>
+      <c r="E29" s="145"/>
+      <c r="F29" s="145"/>
+      <c r="G29" s="145"/>
+      <c r="H29" s="145"/>
+      <c r="I29" s="145"/>
+      <c r="J29" s="145"/>
+      <c r="S29" s="157"/>
+      <c r="T29" s="158"/>
+      <c r="U29" s="149"/>
+      <c r="V29" s="150"/>
+      <c r="W29" s="150"/>
+      <c r="X29" s="150"/>
+      <c r="Y29" s="150"/>
+      <c r="Z29" s="150"/>
+      <c r="AA29" s="151"/>
+      <c r="AC29" s="162"/>
+      <c r="AD29" s="150"/>
+      <c r="AE29" s="150"/>
+      <c r="AF29" s="150"/>
+      <c r="AG29" s="150"/>
+      <c r="AH29" s="150"/>
+      <c r="AI29" s="150"/>
+      <c r="AJ29" s="151"/>
     </row>
     <row r="30" spans="1:36" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="71"/>
       <c r="B30" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="E30" s="143"/>
-      <c r="F30" s="143"/>
-      <c r="G30" s="143"/>
-      <c r="H30" s="143"/>
-      <c r="I30" s="143"/>
-      <c r="J30" s="143"/>
-      <c r="S30" s="155"/>
-      <c r="T30" s="156"/>
-      <c r="U30" s="147"/>
-      <c r="V30" s="148"/>
-      <c r="W30" s="148"/>
-      <c r="X30" s="148"/>
-      <c r="Y30" s="148"/>
-      <c r="Z30" s="148"/>
-      <c r="AA30" s="149"/>
-      <c r="AC30" s="160"/>
-      <c r="AD30" s="148"/>
-      <c r="AE30" s="148"/>
-      <c r="AF30" s="148"/>
-      <c r="AG30" s="148"/>
-      <c r="AH30" s="148"/>
-      <c r="AI30" s="148"/>
-      <c r="AJ30" s="149"/>
+      <c r="E30" s="145"/>
+      <c r="F30" s="145"/>
+      <c r="G30" s="145"/>
+      <c r="H30" s="145"/>
+      <c r="I30" s="145"/>
+      <c r="J30" s="145"/>
+      <c r="S30" s="157"/>
+      <c r="T30" s="158"/>
+      <c r="U30" s="149"/>
+      <c r="V30" s="150"/>
+      <c r="W30" s="150"/>
+      <c r="X30" s="150"/>
+      <c r="Y30" s="150"/>
+      <c r="Z30" s="150"/>
+      <c r="AA30" s="151"/>
+      <c r="AC30" s="162"/>
+      <c r="AD30" s="150"/>
+      <c r="AE30" s="150"/>
+      <c r="AF30" s="150"/>
+      <c r="AG30" s="150"/>
+      <c r="AH30" s="150"/>
+      <c r="AI30" s="150"/>
+      <c r="AJ30" s="151"/>
     </row>
     <row r="31" spans="1:36" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="S31" s="155"/>
-      <c r="T31" s="156"/>
-      <c r="U31" s="147"/>
-      <c r="V31" s="148"/>
-      <c r="W31" s="148"/>
-      <c r="X31" s="148"/>
-      <c r="Y31" s="148"/>
-      <c r="Z31" s="148"/>
-      <c r="AA31" s="149"/>
-      <c r="AC31" s="160"/>
-      <c r="AD31" s="148"/>
-      <c r="AE31" s="148"/>
-      <c r="AF31" s="148"/>
-      <c r="AG31" s="148"/>
-      <c r="AH31" s="148"/>
-      <c r="AI31" s="148"/>
-      <c r="AJ31" s="149"/>
+      <c r="S31" s="157"/>
+      <c r="T31" s="158"/>
+      <c r="U31" s="149"/>
+      <c r="V31" s="150"/>
+      <c r="W31" s="150"/>
+      <c r="X31" s="150"/>
+      <c r="Y31" s="150"/>
+      <c r="Z31" s="150"/>
+      <c r="AA31" s="151"/>
+      <c r="AC31" s="162"/>
+      <c r="AD31" s="150"/>
+      <c r="AE31" s="150"/>
+      <c r="AF31" s="150"/>
+      <c r="AG31" s="150"/>
+      <c r="AH31" s="150"/>
+      <c r="AI31" s="150"/>
+      <c r="AJ31" s="151"/>
     </row>
     <row r="32" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A32" s="72" t="s">
@@ -4051,29 +4128,29 @@
       <c r="F32" s="44"/>
       <c r="G32" s="44"/>
       <c r="H32" s="44"/>
-      <c r="S32" s="165"/>
-      <c r="T32" s="166"/>
-      <c r="U32" s="167"/>
-      <c r="V32" s="168"/>
-      <c r="W32" s="168"/>
-      <c r="X32" s="168"/>
-      <c r="Y32" s="168"/>
-      <c r="Z32" s="168"/>
-      <c r="AA32" s="169"/>
-      <c r="AC32" s="173"/>
-      <c r="AD32" s="168"/>
-      <c r="AE32" s="168"/>
-      <c r="AF32" s="168"/>
-      <c r="AG32" s="168"/>
-      <c r="AH32" s="168"/>
-      <c r="AI32" s="168"/>
-      <c r="AJ32" s="169"/>
+      <c r="S32" s="167"/>
+      <c r="T32" s="168"/>
+      <c r="U32" s="169"/>
+      <c r="V32" s="170"/>
+      <c r="W32" s="170"/>
+      <c r="X32" s="170"/>
+      <c r="Y32" s="170"/>
+      <c r="Z32" s="170"/>
+      <c r="AA32" s="171"/>
+      <c r="AC32" s="175"/>
+      <c r="AD32" s="170"/>
+      <c r="AE32" s="170"/>
+      <c r="AF32" s="170"/>
+      <c r="AG32" s="170"/>
+      <c r="AH32" s="170"/>
+      <c r="AI32" s="170"/>
+      <c r="AJ32" s="171"/>
     </row>
     <row r="33" spans="1:36" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="140" t="s">
+      <c r="A33" s="142" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="140"/>
+      <c r="B33" s="142"/>
       <c r="C33" s="63">
         <f>COUNTIF(D24:AG24,"=8")</f>
         <v>1</v>
@@ -4083,29 +4160,29 @@
       <c r="F33" s="44"/>
       <c r="G33" s="44"/>
       <c r="H33" s="44"/>
-      <c r="S33" s="153" t="s">
+      <c r="S33" s="155" t="s">
         <v>53</v>
       </c>
-      <c r="T33" s="154"/>
-      <c r="U33" s="144" t="s">
+      <c r="T33" s="156"/>
+      <c r="U33" s="146" t="s">
         <v>54</v>
       </c>
-      <c r="V33" s="145"/>
-      <c r="W33" s="145"/>
-      <c r="X33" s="145"/>
-      <c r="Y33" s="145"/>
-      <c r="Z33" s="145"/>
-      <c r="AA33" s="146"/>
-      <c r="AC33" s="159" t="s">
+      <c r="V33" s="147"/>
+      <c r="W33" s="147"/>
+      <c r="X33" s="147"/>
+      <c r="Y33" s="147"/>
+      <c r="Z33" s="147"/>
+      <c r="AA33" s="148"/>
+      <c r="AC33" s="161" t="s">
         <v>55</v>
       </c>
-      <c r="AD33" s="145"/>
-      <c r="AE33" s="145"/>
-      <c r="AF33" s="145"/>
-      <c r="AG33" s="145"/>
-      <c r="AH33" s="145"/>
-      <c r="AI33" s="145"/>
-      <c r="AJ33" s="146"/>
+      <c r="AD33" s="147"/>
+      <c r="AE33" s="147"/>
+      <c r="AF33" s="147"/>
+      <c r="AG33" s="147"/>
+      <c r="AH33" s="147"/>
+      <c r="AI33" s="147"/>
+      <c r="AJ33" s="148"/>
     </row>
     <row r="34" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A34" s="63" t="s">
@@ -4121,23 +4198,23 @@
       <c r="F34" s="44"/>
       <c r="G34" s="44"/>
       <c r="H34" s="44"/>
-      <c r="S34" s="155"/>
-      <c r="T34" s="156"/>
-      <c r="U34" s="147"/>
-      <c r="V34" s="148"/>
-      <c r="W34" s="148"/>
-      <c r="X34" s="148"/>
-      <c r="Y34" s="148"/>
-      <c r="Z34" s="148"/>
-      <c r="AA34" s="149"/>
-      <c r="AC34" s="160"/>
-      <c r="AD34" s="148"/>
-      <c r="AE34" s="148"/>
-      <c r="AF34" s="148"/>
-      <c r="AG34" s="148"/>
-      <c r="AH34" s="148"/>
-      <c r="AI34" s="148"/>
-      <c r="AJ34" s="149"/>
+      <c r="S34" s="157"/>
+      <c r="T34" s="158"/>
+      <c r="U34" s="149"/>
+      <c r="V34" s="150"/>
+      <c r="W34" s="150"/>
+      <c r="X34" s="150"/>
+      <c r="Y34" s="150"/>
+      <c r="Z34" s="150"/>
+      <c r="AA34" s="151"/>
+      <c r="AC34" s="162"/>
+      <c r="AD34" s="150"/>
+      <c r="AE34" s="150"/>
+      <c r="AF34" s="150"/>
+      <c r="AG34" s="150"/>
+      <c r="AH34" s="150"/>
+      <c r="AI34" s="150"/>
+      <c r="AJ34" s="151"/>
     </row>
     <row r="35" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A35" s="63" t="s">
@@ -4153,23 +4230,23 @@
       <c r="F35" s="44"/>
       <c r="G35" s="44"/>
       <c r="H35" s="44"/>
-      <c r="S35" s="155"/>
-      <c r="T35" s="156"/>
-      <c r="U35" s="147"/>
-      <c r="V35" s="148"/>
-      <c r="W35" s="148"/>
-      <c r="X35" s="148"/>
-      <c r="Y35" s="148"/>
-      <c r="Z35" s="148"/>
-      <c r="AA35" s="149"/>
-      <c r="AC35" s="160"/>
-      <c r="AD35" s="148"/>
-      <c r="AE35" s="148"/>
-      <c r="AF35" s="148"/>
-      <c r="AG35" s="148"/>
-      <c r="AH35" s="148"/>
-      <c r="AI35" s="148"/>
-      <c r="AJ35" s="149"/>
+      <c r="S35" s="157"/>
+      <c r="T35" s="158"/>
+      <c r="U35" s="149"/>
+      <c r="V35" s="150"/>
+      <c r="W35" s="150"/>
+      <c r="X35" s="150"/>
+      <c r="Y35" s="150"/>
+      <c r="Z35" s="150"/>
+      <c r="AA35" s="151"/>
+      <c r="AC35" s="162"/>
+      <c r="AD35" s="150"/>
+      <c r="AE35" s="150"/>
+      <c r="AF35" s="150"/>
+      <c r="AG35" s="150"/>
+      <c r="AH35" s="150"/>
+      <c r="AI35" s="150"/>
+      <c r="AJ35" s="151"/>
     </row>
     <row r="36" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A36" s="63" t="s">
@@ -4185,29 +4262,29 @@
       <c r="F36" s="44"/>
       <c r="G36" s="44"/>
       <c r="H36" s="44"/>
-      <c r="S36" s="155"/>
-      <c r="T36" s="156"/>
-      <c r="U36" s="147"/>
-      <c r="V36" s="148"/>
-      <c r="W36" s="148"/>
-      <c r="X36" s="148"/>
-      <c r="Y36" s="148"/>
-      <c r="Z36" s="148"/>
-      <c r="AA36" s="149"/>
-      <c r="AC36" s="160"/>
-      <c r="AD36" s="148"/>
-      <c r="AE36" s="148"/>
-      <c r="AF36" s="148"/>
-      <c r="AG36" s="148"/>
-      <c r="AH36" s="148"/>
-      <c r="AI36" s="148"/>
-      <c r="AJ36" s="149"/>
+      <c r="S36" s="157"/>
+      <c r="T36" s="158"/>
+      <c r="U36" s="149"/>
+      <c r="V36" s="150"/>
+      <c r="W36" s="150"/>
+      <c r="X36" s="150"/>
+      <c r="Y36" s="150"/>
+      <c r="Z36" s="150"/>
+      <c r="AA36" s="151"/>
+      <c r="AC36" s="162"/>
+      <c r="AD36" s="150"/>
+      <c r="AE36" s="150"/>
+      <c r="AF36" s="150"/>
+      <c r="AG36" s="150"/>
+      <c r="AH36" s="150"/>
+      <c r="AI36" s="150"/>
+      <c r="AJ36" s="151"/>
     </row>
     <row r="37" spans="1:36" ht="38.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="174" t="s">
+      <c r="A37" s="176" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="174"/>
+      <c r="B37" s="176"/>
       <c r="C37" s="63">
         <f>COUNTIF(D25:AG25,"&gt;0")</f>
         <v>20</v>
@@ -4217,23 +4294,23 @@
       <c r="F37" s="44"/>
       <c r="G37" s="44"/>
       <c r="H37" s="44"/>
-      <c r="S37" s="157"/>
-      <c r="T37" s="158"/>
-      <c r="U37" s="150"/>
-      <c r="V37" s="151"/>
-      <c r="W37" s="151"/>
-      <c r="X37" s="151"/>
-      <c r="Y37" s="151"/>
-      <c r="Z37" s="151"/>
-      <c r="AA37" s="152"/>
-      <c r="AC37" s="161"/>
-      <c r="AD37" s="151"/>
-      <c r="AE37" s="151"/>
-      <c r="AF37" s="151"/>
-      <c r="AG37" s="151"/>
-      <c r="AH37" s="151"/>
-      <c r="AI37" s="151"/>
-      <c r="AJ37" s="152"/>
+      <c r="S37" s="159"/>
+      <c r="T37" s="160"/>
+      <c r="U37" s="152"/>
+      <c r="V37" s="153"/>
+      <c r="W37" s="153"/>
+      <c r="X37" s="153"/>
+      <c r="Y37" s="153"/>
+      <c r="Z37" s="153"/>
+      <c r="AA37" s="154"/>
+      <c r="AC37" s="163"/>
+      <c r="AD37" s="153"/>
+      <c r="AE37" s="153"/>
+      <c r="AF37" s="153"/>
+      <c r="AG37" s="153"/>
+      <c r="AH37" s="153"/>
+      <c r="AI37" s="153"/>
+      <c r="AJ37" s="154"/>
     </row>
     <row r="38" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A38" s="63" t="s">
@@ -4273,10 +4350,10 @@
       <c r="H40" s="44"/>
     </row>
     <row r="41" spans="1:36" ht="35.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="174" t="s">
+      <c r="A41" s="176" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="174"/>
+      <c r="B41" s="176"/>
       <c r="C41" s="63">
         <f>AH25</f>
         <v>160</v>
@@ -4288,10 +4365,10 @@
       <c r="H41" s="44"/>
     </row>
     <row r="42" spans="1:36" ht="38.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="174" t="s">
+      <c r="A42" s="176" t="s">
         <v>63</v>
       </c>
-      <c r="B42" s="174"/>
+      <c r="B42" s="176"/>
       <c r="C42" s="63">
         <v>45</v>
       </c>
@@ -4485,10 +4562,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA136F23-B726-450C-8838-7114D5303DC9}">
-  <dimension ref="A1:AJ53"/>
+  <dimension ref="A1:AJ67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="X23" sqref="X23"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
+      <selection activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4497,11 +4574,14 @@
     <col min="2" max="2" width="33.1796875" style="45" customWidth="1"/>
     <col min="3" max="3" width="10.54296875" style="42" customWidth="1"/>
     <col min="4" max="4" width="9.54296875" style="4" customWidth="1"/>
-    <col min="5" max="8" width="6.81640625" style="4" customWidth="1"/>
-    <col min="9" max="10" width="6.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="6.81640625" style="4" customWidth="1"/>
-    <col min="13" max="33" width="7.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.81640625" style="4" customWidth="1"/>
+    <col min="5" max="7" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6328125" style="4" customWidth="1"/>
+    <col min="9" max="10" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.26953125" style="4" customWidth="1"/>
+    <col min="12" max="14" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="32" width="7.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.54296875" style="4" customWidth="1"/>
+    <col min="34" max="34" width="7.54296875" style="4" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="7.1796875" style="4" customWidth="1"/>
     <col min="36" max="36" width="11.54296875" style="4" customWidth="1"/>
     <col min="37" max="16384" width="8.7265625" style="4"/>
@@ -4604,7 +4684,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="82" t="s">
-        <v>7</v>
+        <v>163</v>
       </c>
       <c r="C5" s="76"/>
       <c r="D5" s="83" t="s">
@@ -4613,7 +4693,7 @@
       <c r="E5" s="78"/>
       <c r="F5" s="78"/>
       <c r="H5" s="84" t="s">
-        <v>70</v>
+        <v>165</v>
       </c>
       <c r="I5" s="84"/>
       <c r="J5" s="78"/>
@@ -4622,19 +4702,19 @@
       </c>
       <c r="L5" s="78"/>
       <c r="M5" s="78"/>
-      <c r="N5" s="142" t="s">
-        <v>11</v>
-      </c>
-      <c r="O5" s="142"/>
-      <c r="P5" s="142"/>
-      <c r="Q5" s="142"/>
+      <c r="N5" s="144" t="s">
+        <v>167</v>
+      </c>
+      <c r="O5" s="144"/>
+      <c r="P5" s="144"/>
+      <c r="Q5" s="144"/>
     </row>
     <row r="6" spans="1:36" ht="17" x14ac:dyDescent="0.4">
       <c r="A6" s="74" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="82" t="s">
-        <v>13</v>
+        <v>164</v>
       </c>
       <c r="C6" s="76"/>
       <c r="D6" s="83" t="s">
@@ -4643,7 +4723,7 @@
       <c r="E6" s="78"/>
       <c r="F6" s="78"/>
       <c r="H6" s="84" t="s">
-        <v>71</v>
+        <v>166</v>
       </c>
       <c r="I6" s="84"/>
       <c r="J6" s="78"/>
@@ -4652,12 +4732,12 @@
       </c>
       <c r="L6" s="87"/>
       <c r="M6" s="76"/>
-      <c r="N6" s="141" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" s="141"/>
-      <c r="P6" s="141"/>
-      <c r="Q6" s="141"/>
+      <c r="N6" s="143" t="s">
+        <v>168</v>
+      </c>
+      <c r="O6" s="143"/>
+      <c r="P6" s="143"/>
+      <c r="Q6" s="143"/>
       <c r="W6"/>
     </row>
     <row r="7" spans="1:36" s="42" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -4680,13 +4760,13 @@
       <c r="Q7" s="76"/>
     </row>
     <row r="9" spans="1:36" ht="17" x14ac:dyDescent="0.35">
-      <c r="A9" s="175" t="s">
+      <c r="A9" s="177" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="139" t="s">
+      <c r="B9" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="175" t="s">
+      <c r="C9" s="177" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="50" t="str">
@@ -4813,7 +4893,7 @@
         <f t="shared" si="0"/>
         <v>Sun</v>
       </c>
-      <c r="AI9" s="139" t="s">
+      <c r="AI9" s="141" t="s">
         <v>23</v>
       </c>
       <c r="AJ9" s="90" t="s">
@@ -4821,9 +4901,9 @@
       </c>
     </row>
     <row r="10" spans="1:36" ht="17" x14ac:dyDescent="0.35">
-      <c r="A10" s="175"/>
-      <c r="B10" s="139"/>
-      <c r="C10" s="175"/>
+      <c r="A10" s="177"/>
+      <c r="B10" s="141"/>
+      <c r="C10" s="177"/>
       <c r="D10" s="51" cm="1">
         <f t="array" ref="D10:AH10">IFERROR(IF(OR((B3-B2+1)&gt;31,B2="",B3=""),"",_xlfn.SEQUENCE(,B3-B2+1,B2)),"")</f>
         <v>45646</v>
@@ -4918,7 +4998,7 @@
       <c r="AH10" s="51">
         <v>45676</v>
       </c>
-      <c r="AI10" s="139"/>
+      <c r="AI10" s="141"/>
       <c r="AJ10" s="90"/>
     </row>
     <row r="11" spans="1:36" ht="17" x14ac:dyDescent="0.4">
@@ -4961,255 +5041,218 @@
       <c r="AI11" s="55"/>
       <c r="AJ11" s="73"/>
     </row>
-    <row r="12" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A12" s="88" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="89" t="s">
-        <v>27</v>
+    <row r="12" spans="1:36" ht="68" x14ac:dyDescent="0.4">
+      <c r="A12" s="184" t="s">
+        <v>182</v>
+      </c>
+      <c r="B12" s="139" t="s">
+        <v>171</v>
       </c>
       <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57">
-        <v>0</v>
-      </c>
-      <c r="F12" s="57">
-        <v>0</v>
-      </c>
-      <c r="G12" s="50">
-        <v>8</v>
+      <c r="D12" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57">
+        <v>0.5</v>
       </c>
       <c r="H12" s="57">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="I12" s="50"/>
       <c r="J12" s="50"/>
       <c r="K12" s="50">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="L12" s="50"/>
-      <c r="M12" s="50">
-        <v>3</v>
-      </c>
+      <c r="M12" s="50"/>
       <c r="N12" s="50">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="O12" s="50">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="P12" s="50"/>
-      <c r="Q12" s="50"/>
-      <c r="R12" s="50">
-        <v>2</v>
-      </c>
+      <c r="Q12" s="50">
+        <v>0.2</v>
+      </c>
+      <c r="R12" s="50"/>
       <c r="S12" s="50"/>
-      <c r="T12" s="50">
-        <v>0</v>
-      </c>
-      <c r="U12" s="50">
-        <v>2</v>
-      </c>
-      <c r="V12" s="50">
-        <v>1</v>
-      </c>
-      <c r="W12" s="50">
-        <v>1</v>
-      </c>
+      <c r="T12" s="50"/>
+      <c r="U12" s="50"/>
+      <c r="V12" s="50"/>
+      <c r="W12" s="50"/>
       <c r="X12" s="50"/>
-      <c r="Y12" s="50">
-        <v>2</v>
-      </c>
-      <c r="Z12" s="50">
-        <v>4</v>
-      </c>
-      <c r="AA12" s="50">
-        <v>1</v>
-      </c>
-      <c r="AB12" s="50">
-        <v>3</v>
-      </c>
+      <c r="Y12" s="50"/>
+      <c r="Z12" s="50"/>
+      <c r="AA12" s="50"/>
+      <c r="AB12" s="50"/>
       <c r="AC12" s="50"/>
-      <c r="AD12" s="50">
-        <v>1</v>
-      </c>
+      <c r="AD12" s="50"/>
       <c r="AE12" s="50"/>
       <c r="AF12" s="57"/>
-      <c r="AG12" s="57">
-        <v>1</v>
-      </c>
+      <c r="AG12" s="57"/>
       <c r="AH12" s="57"/>
       <c r="AI12" s="58">
         <f>SUM(D12:AH12)</f>
-        <v>43</v>
+        <v>3.2</v>
       </c>
       <c r="AJ12" s="73"/>
     </row>
-    <row r="13" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="B13" s="89" t="s">
-        <v>28</v>
+    <row r="13" spans="1:36" ht="68" x14ac:dyDescent="0.4">
+      <c r="A13" s="185"/>
+      <c r="B13" s="139" t="s">
+        <v>172</v>
       </c>
       <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
+      <c r="D13" s="57">
+        <v>0.5</v>
+      </c>
       <c r="E13" s="57"/>
       <c r="F13" s="57"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="57"/>
+      <c r="G13" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="H13" s="57">
+        <v>0.5</v>
+      </c>
       <c r="I13" s="50"/>
       <c r="J13" s="50"/>
       <c r="K13" s="50">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L13" s="50"/>
-      <c r="M13" s="50">
-        <v>1</v>
-      </c>
+      <c r="M13" s="50"/>
       <c r="N13" s="50">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="O13" s="50">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="P13" s="50"/>
-      <c r="Q13" s="50"/>
+      <c r="Q13" s="50">
+        <v>0.8</v>
+      </c>
       <c r="R13" s="50">
-        <v>4</v>
+        <v>0.2</v>
       </c>
       <c r="S13" s="50"/>
       <c r="T13" s="50"/>
-      <c r="U13" s="50">
-        <v>4</v>
-      </c>
-      <c r="V13" s="50">
-        <v>4</v>
-      </c>
-      <c r="W13" s="50">
-        <v>4</v>
-      </c>
+      <c r="U13" s="50"/>
+      <c r="V13" s="50"/>
+      <c r="W13" s="50"/>
       <c r="X13" s="50"/>
-      <c r="Y13" s="50">
-        <v>3</v>
-      </c>
-      <c r="Z13" s="50">
-        <v>2</v>
-      </c>
-      <c r="AA13" s="50">
-        <v>2</v>
-      </c>
-      <c r="AB13" s="50">
-        <v>3</v>
-      </c>
-      <c r="AC13" s="50">
-        <v>5</v>
-      </c>
-      <c r="AD13" s="50">
-        <v>2</v>
-      </c>
+      <c r="Y13" s="50"/>
+      <c r="Z13" s="50"/>
+      <c r="AA13" s="50"/>
+      <c r="AB13" s="50"/>
+      <c r="AC13" s="50"/>
+      <c r="AD13" s="50"/>
       <c r="AE13" s="50"/>
       <c r="AF13" s="57"/>
-      <c r="AG13" s="57">
-        <v>3</v>
-      </c>
+      <c r="AG13" s="57"/>
       <c r="AH13" s="57"/>
       <c r="AI13" s="58">
         <f>SUM(D13:AH13)</f>
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="AJ13" s="73"/>
     </row>
-    <row r="14" spans="1:36" ht="34" x14ac:dyDescent="0.4">
-      <c r="A14" s="89" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="89" t="s">
-        <v>30</v>
+    <row r="14" spans="1:36" ht="68" x14ac:dyDescent="0.4">
+      <c r="A14" s="185"/>
+      <c r="B14" s="139" t="s">
+        <v>173</v>
       </c>
       <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
+      <c r="D14" s="57">
+        <v>0.5</v>
+      </c>
       <c r="E14" s="57"/>
       <c r="F14" s="57"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="57"/>
+      <c r="G14" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="H14" s="57">
+        <v>0.5</v>
+      </c>
       <c r="I14" s="50"/>
       <c r="J14" s="50"/>
       <c r="K14" s="50">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="L14" s="50"/>
-      <c r="M14" s="50">
-        <v>1</v>
-      </c>
+      <c r="M14" s="50"/>
       <c r="N14" s="50">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O14" s="50">
-        <v>1</v>
-      </c>
-      <c r="P14" s="50">
-        <v>6</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="P14" s="50"/>
       <c r="Q14" s="50"/>
       <c r="R14" s="50">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="S14" s="50"/>
       <c r="T14" s="50"/>
-      <c r="U14" s="50">
-        <v>1</v>
-      </c>
-      <c r="V14" s="50">
-        <v>1</v>
-      </c>
-      <c r="W14" s="50">
-        <v>1</v>
-      </c>
+      <c r="U14" s="50"/>
+      <c r="V14" s="50"/>
+      <c r="W14" s="50"/>
       <c r="X14" s="50"/>
-      <c r="Y14" s="50">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="50">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="50">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="50">
-        <v>5</v>
-      </c>
+      <c r="Y14" s="50"/>
+      <c r="Z14" s="50"/>
+      <c r="AA14" s="50"/>
+      <c r="AB14" s="50"/>
       <c r="AC14" s="50"/>
-      <c r="AD14" s="50">
-        <v>0</v>
-      </c>
+      <c r="AD14" s="50"/>
       <c r="AE14" s="50"/>
       <c r="AF14" s="57"/>
-      <c r="AG14" s="57">
-        <v>2</v>
-      </c>
+      <c r="AG14" s="57"/>
       <c r="AH14" s="57"/>
       <c r="AI14" s="58">
         <f>SUM(D14:AH14)</f>
-        <v>22</v>
+        <v>3.2</v>
       </c>
       <c r="AJ14" s="73"/>
     </row>
-    <row r="15" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A15" s="67"/>
-      <c r="B15" s="56"/>
+    <row r="15" spans="1:36" ht="68" x14ac:dyDescent="0.4">
+      <c r="A15" s="185"/>
+      <c r="B15" s="139" t="s">
+        <v>174</v>
+      </c>
       <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
+      <c r="D15" s="57">
+        <v>1.5</v>
+      </c>
       <c r="E15" s="57"/>
       <c r="F15" s="57"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="57"/>
+      <c r="G15" s="57">
+        <v>1.5</v>
+      </c>
+      <c r="H15" s="57">
+        <v>1.5</v>
+      </c>
       <c r="I15" s="50"/>
       <c r="J15" s="50"/>
-      <c r="K15" s="50"/>
+      <c r="K15" s="50">
+        <v>1.5</v>
+      </c>
       <c r="L15" s="50"/>
       <c r="M15" s="50"/>
-      <c r="N15" s="50"/>
-      <c r="O15" s="50"/>
+      <c r="N15" s="50">
+        <v>1.5</v>
+      </c>
+      <c r="O15" s="50">
+        <v>1.5</v>
+      </c>
       <c r="P15" s="50"/>
-      <c r="Q15" s="50"/>
-      <c r="R15" s="50"/>
+      <c r="Q15" s="50">
+        <v>1</v>
+      </c>
+      <c r="R15" s="50">
+        <v>1</v>
+      </c>
       <c r="S15" s="50"/>
       <c r="T15" s="50"/>
       <c r="U15" s="50"/>
@@ -5226,28 +5269,47 @@
       <c r="AF15" s="57"/>
       <c r="AG15" s="57"/>
       <c r="AH15" s="57"/>
-      <c r="AI15" s="58"/>
+      <c r="AI15" s="58">
+        <f t="shared" ref="AI15:AI17" si="1">SUM(D15:AH15)</f>
+        <v>11</v>
+      </c>
       <c r="AJ15" s="73"/>
     </row>
-    <row r="16" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A16" s="67"/>
-      <c r="B16" s="56"/>
+    <row r="16" spans="1:36" ht="85" x14ac:dyDescent="0.4">
+      <c r="A16" s="185"/>
+      <c r="B16" s="139" t="s">
+        <v>175</v>
+      </c>
       <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
+      <c r="D16" s="57">
+        <v>1.5</v>
+      </c>
       <c r="E16" s="57"/>
       <c r="F16" s="57"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="57"/>
+      <c r="G16" s="57">
+        <v>1.5</v>
+      </c>
+      <c r="H16" s="57">
+        <v>1.5</v>
+      </c>
       <c r="I16" s="50"/>
       <c r="J16" s="50"/>
-      <c r="K16" s="50"/>
+      <c r="K16" s="50">
+        <v>1.5</v>
+      </c>
       <c r="L16" s="50"/>
       <c r="M16" s="50"/>
-      <c r="N16" s="50"/>
-      <c r="O16" s="50"/>
+      <c r="N16" s="50">
+        <v>1.5</v>
+      </c>
+      <c r="O16" s="50">
+        <v>1.5</v>
+      </c>
       <c r="P16" s="50"/>
       <c r="Q16" s="50"/>
-      <c r="R16" s="50"/>
+      <c r="R16" s="50">
+        <v>0.6</v>
+      </c>
       <c r="S16" s="50"/>
       <c r="T16" s="50"/>
       <c r="U16" s="50"/>
@@ -5264,148 +5326,135 @@
       <c r="AF16" s="57"/>
       <c r="AG16" s="57"/>
       <c r="AH16" s="57"/>
-      <c r="AI16" s="58"/>
+      <c r="AI16" s="58">
+        <f t="shared" si="1"/>
+        <v>9.6</v>
+      </c>
       <c r="AJ16" s="73"/>
     </row>
-    <row r="17" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A17" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="59"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="54"/>
-      <c r="M17" s="54"/>
-      <c r="N17" s="54"/>
-      <c r="O17" s="54"/>
-      <c r="P17" s="54"/>
-      <c r="Q17" s="54"/>
-      <c r="R17" s="54"/>
-      <c r="S17" s="54"/>
-      <c r="T17" s="54"/>
-      <c r="U17" s="54"/>
-      <c r="V17" s="54"/>
-      <c r="W17" s="54"/>
-      <c r="X17" s="54"/>
-      <c r="Y17" s="54"/>
-      <c r="Z17" s="54"/>
-      <c r="AA17" s="54"/>
-      <c r="AB17" s="54"/>
-      <c r="AC17" s="54"/>
-      <c r="AD17" s="54"/>
-      <c r="AE17" s="54"/>
-      <c r="AF17" s="54"/>
-      <c r="AG17" s="54"/>
-      <c r="AH17" s="54"/>
-      <c r="AI17" s="55"/>
+    <row r="17" spans="1:36" ht="102" x14ac:dyDescent="0.4">
+      <c r="A17" s="185"/>
+      <c r="B17" s="139" t="s">
+        <v>176</v>
+      </c>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57">
+        <v>1.5</v>
+      </c>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57">
+        <v>1.5</v>
+      </c>
+      <c r="H17" s="57">
+        <v>1.5</v>
+      </c>
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="50">
+        <v>1.5</v>
+      </c>
+      <c r="L17" s="50"/>
+      <c r="M17" s="50"/>
+      <c r="N17" s="50">
+        <v>1.5</v>
+      </c>
+      <c r="O17" s="50">
+        <v>1.5</v>
+      </c>
+      <c r="P17" s="50"/>
+      <c r="Q17" s="50"/>
+      <c r="R17" s="50"/>
+      <c r="S17" s="50"/>
+      <c r="T17" s="50"/>
+      <c r="U17" s="50"/>
+      <c r="V17" s="50"/>
+      <c r="W17" s="50"/>
+      <c r="X17" s="50"/>
+      <c r="Y17" s="50"/>
+      <c r="Z17" s="50"/>
+      <c r="AA17" s="50"/>
+      <c r="AB17" s="50"/>
+      <c r="AC17" s="50"/>
+      <c r="AD17" s="50"/>
+      <c r="AE17" s="50"/>
+      <c r="AF17" s="57"/>
+      <c r="AG17" s="57"/>
+      <c r="AH17" s="57"/>
+      <c r="AI17" s="58">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
       <c r="AJ17" s="73"/>
     </row>
-    <row r="18" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A18" s="67"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="57" t="s">
-        <v>34</v>
-      </c>
+    <row r="18" spans="1:36" ht="136" x14ac:dyDescent="0.4">
+      <c r="A18" s="185"/>
+      <c r="B18" s="139" t="s">
+        <v>177</v>
+      </c>
+      <c r="C18" s="57"/>
       <c r="D18" s="57"/>
-      <c r="E18" s="57">
-        <v>0</v>
-      </c>
-      <c r="F18" s="57">
-        <v>0</v>
-      </c>
-      <c r="G18" s="50"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57">
+        <v>0.5</v>
+      </c>
       <c r="H18" s="57">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="I18" s="50"/>
       <c r="J18" s="50"/>
-      <c r="K18" s="50">
-        <v>1</v>
-      </c>
+      <c r="K18" s="50"/>
       <c r="L18" s="50"/>
-      <c r="M18" s="50">
-        <v>2</v>
-      </c>
+      <c r="M18" s="50"/>
       <c r="N18" s="50"/>
       <c r="O18" s="50"/>
       <c r="P18" s="50"/>
       <c r="Q18" s="50"/>
-      <c r="R18" s="50">
-        <v>1</v>
-      </c>
+      <c r="R18" s="50"/>
       <c r="S18" s="50"/>
       <c r="T18" s="50"/>
-      <c r="U18" s="50">
-        <v>1</v>
-      </c>
-      <c r="V18" s="50">
-        <v>2</v>
-      </c>
-      <c r="W18" s="50">
-        <v>2</v>
-      </c>
+      <c r="U18" s="50"/>
+      <c r="V18" s="50"/>
+      <c r="W18" s="50"/>
       <c r="X18" s="50"/>
-      <c r="Y18" s="50">
-        <v>1</v>
-      </c>
-      <c r="Z18" s="50">
-        <v>2</v>
-      </c>
-      <c r="AA18" s="50">
-        <v>4</v>
-      </c>
-      <c r="AB18" s="50">
-        <v>2</v>
-      </c>
+      <c r="Y18" s="50"/>
+      <c r="Z18" s="50"/>
+      <c r="AA18" s="50"/>
+      <c r="AB18" s="50"/>
       <c r="AC18" s="50"/>
-      <c r="AD18" s="50">
-        <v>4</v>
-      </c>
+      <c r="AD18" s="50"/>
       <c r="AE18" s="50"/>
       <c r="AF18" s="57"/>
       <c r="AG18" s="57"/>
       <c r="AH18" s="57"/>
-      <c r="AI18" s="58">
-        <f>SUM(D18:AH18)</f>
-        <v>25</v>
-      </c>
+      <c r="AI18" s="58"/>
       <c r="AJ18" s="73"/>
     </row>
-    <row r="19" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A19" s="67"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="57" t="s">
-        <v>36</v>
-      </c>
+    <row r="19" spans="1:36" ht="136" x14ac:dyDescent="0.4">
+      <c r="A19" s="185"/>
+      <c r="B19" s="139" t="s">
+        <v>178</v>
+      </c>
+      <c r="C19" s="57"/>
       <c r="D19" s="57"/>
       <c r="E19" s="57"/>
       <c r="F19" s="57"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="50">
-        <v>2</v>
-      </c>
+      <c r="G19" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="H19" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="I19" s="50"/>
       <c r="J19" s="50"/>
-      <c r="K19" s="50">
-        <v>1</v>
-      </c>
+      <c r="K19" s="50"/>
       <c r="L19" s="50"/>
       <c r="M19" s="50"/>
       <c r="N19" s="50"/>
       <c r="O19" s="50"/>
-      <c r="P19" s="50">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="50">
-        <v>1</v>
-      </c>
+      <c r="P19" s="50"/>
+      <c r="Q19" s="50"/>
       <c r="R19" s="50"/>
       <c r="S19" s="50"/>
       <c r="T19" s="50"/>
@@ -5413,12 +5462,8 @@
       <c r="V19" s="50"/>
       <c r="W19" s="50"/>
       <c r="X19" s="50"/>
-      <c r="Y19" s="50">
-        <v>1</v>
-      </c>
-      <c r="Z19" s="50">
-        <v>1</v>
-      </c>
+      <c r="Y19" s="50"/>
+      <c r="Z19" s="50"/>
       <c r="AA19" s="50"/>
       <c r="AB19" s="50"/>
       <c r="AC19" s="50"/>
@@ -5427,44 +5472,29 @@
       <c r="AF19" s="57"/>
       <c r="AG19" s="57"/>
       <c r="AH19" s="57"/>
-      <c r="AI19" s="58">
-        <f>SUM(D19:AH19)</f>
-        <v>7</v>
-      </c>
+      <c r="AI19" s="58"/>
       <c r="AJ19" s="73"/>
     </row>
-    <row r="20" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A20" s="67"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="57" t="s">
-        <v>37</v>
-      </c>
+    <row r="20" spans="1:36" ht="136" x14ac:dyDescent="0.4">
+      <c r="A20" s="185"/>
+      <c r="B20" s="139" t="s">
+        <v>179</v>
+      </c>
+      <c r="C20" s="57"/>
       <c r="D20" s="57"/>
       <c r="E20" s="57"/>
       <c r="F20" s="57"/>
       <c r="G20" s="50"/>
       <c r="H20" s="57"/>
-      <c r="I20" s="50">
-        <v>2</v>
-      </c>
+      <c r="I20" s="50"/>
       <c r="J20" s="50"/>
-      <c r="K20" s="50">
-        <v>2</v>
-      </c>
+      <c r="K20" s="50"/>
       <c r="L20" s="50"/>
-      <c r="M20" s="50">
-        <v>1</v>
-      </c>
-      <c r="N20" s="50">
-        <v>3</v>
-      </c>
+      <c r="M20" s="50"/>
+      <c r="N20" s="50"/>
       <c r="O20" s="50"/>
-      <c r="P20" s="50">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="50">
-        <v>1</v>
-      </c>
+      <c r="P20" s="50"/>
+      <c r="Q20" s="50"/>
       <c r="R20" s="50"/>
       <c r="S20" s="50"/>
       <c r="T20" s="50"/>
@@ -5472,76 +5502,71 @@
       <c r="V20" s="50"/>
       <c r="W20" s="50"/>
       <c r="X20" s="50"/>
-      <c r="Y20" s="50">
-        <v>3</v>
-      </c>
-      <c r="Z20" s="50">
-        <v>1</v>
-      </c>
-      <c r="AA20" s="50">
-        <v>1</v>
-      </c>
+      <c r="Y20" s="50"/>
+      <c r="Z20" s="50"/>
+      <c r="AA20" s="50"/>
       <c r="AB20" s="50"/>
       <c r="AC20" s="50"/>
-      <c r="AD20" s="50">
-        <v>1</v>
-      </c>
+      <c r="AD20" s="50"/>
       <c r="AE20" s="50"/>
       <c r="AF20" s="57"/>
-      <c r="AG20" s="57">
-        <v>2</v>
-      </c>
+      <c r="AG20" s="57"/>
       <c r="AH20" s="57"/>
-      <c r="AI20" s="58">
-        <f>SUM(D20:AH20)</f>
-        <v>18</v>
-      </c>
+      <c r="AI20" s="58"/>
       <c r="AJ20" s="73"/>
     </row>
-    <row r="21" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="68"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="61"/>
-      <c r="H21" s="61"/>
-      <c r="I21" s="61"/>
-      <c r="J21" s="61"/>
-      <c r="K21" s="61"/>
-      <c r="L21" s="61"/>
-      <c r="M21" s="61"/>
-      <c r="N21" s="61"/>
-      <c r="O21" s="61"/>
-      <c r="P21" s="61"/>
-      <c r="Q21" s="61"/>
-      <c r="R21" s="61"/>
-      <c r="S21" s="61"/>
-      <c r="T21" s="61"/>
-      <c r="U21" s="61"/>
-      <c r="V21" s="61"/>
-      <c r="W21" s="61"/>
-      <c r="X21" s="61"/>
-      <c r="Y21" s="61"/>
-      <c r="Z21" s="61"/>
-      <c r="AA21" s="61"/>
-      <c r="AB21" s="61"/>
-      <c r="AC21" s="61"/>
-      <c r="AD21" s="61"/>
-      <c r="AE21" s="61"/>
-      <c r="AF21" s="61"/>
-      <c r="AG21" s="62"/>
-      <c r="AH21" s="62"/>
-      <c r="AI21" s="62"/>
+    <row r="21" spans="1:36" ht="228" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="186"/>
+      <c r="B21" s="139" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57">
+        <v>1</v>
+      </c>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="50">
+        <v>1</v>
+      </c>
+      <c r="L21" s="50"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="50">
+        <v>1</v>
+      </c>
+      <c r="O21" s="50">
+        <v>1</v>
+      </c>
+      <c r="P21" s="50"/>
+      <c r="Q21" s="50"/>
+      <c r="R21" s="50"/>
+      <c r="S21" s="50"/>
+      <c r="T21" s="50"/>
+      <c r="U21" s="50"/>
+      <c r="V21" s="50"/>
+      <c r="W21" s="50"/>
+      <c r="X21" s="50"/>
+      <c r="Y21" s="50"/>
+      <c r="Z21" s="50"/>
+      <c r="AA21" s="50"/>
+      <c r="AB21" s="50"/>
+      <c r="AC21" s="50"/>
+      <c r="AD21" s="50"/>
+      <c r="AE21" s="50"/>
+      <c r="AF21" s="57"/>
+      <c r="AG21" s="57"/>
+      <c r="AH21" s="57"/>
+      <c r="AI21" s="58"/>
       <c r="AJ21" s="73"/>
     </row>
     <row r="22" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A22" s="176" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="177"/>
-      <c r="C22" s="178"/>
+      <c r="A22" s="140"/>
+      <c r="B22" s="139"/>
+      <c r="C22" s="57"/>
       <c r="D22" s="57"/>
       <c r="E22" s="57"/>
       <c r="F22" s="57"/>
@@ -5573,18 +5598,13 @@
       <c r="AF22" s="57"/>
       <c r="AG22" s="57"/>
       <c r="AH22" s="57"/>
-      <c r="AI22" s="58">
-        <f>SUM(D22:AH22)</f>
-        <v>0</v>
-      </c>
+      <c r="AI22" s="58"/>
       <c r="AJ22" s="73"/>
     </row>
     <row r="23" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A23" s="176" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="177"/>
-      <c r="C23" s="178"/>
+      <c r="A23" s="140"/>
+      <c r="B23" s="139"/>
+      <c r="C23" s="57"/>
       <c r="D23" s="57"/>
       <c r="E23" s="57"/>
       <c r="F23" s="57"/>
@@ -5616,18 +5636,13 @@
       <c r="AF23" s="57"/>
       <c r="AG23" s="57"/>
       <c r="AH23" s="57"/>
-      <c r="AI23" s="58">
-        <f>SUM(D23:AH23)</f>
-        <v>0</v>
-      </c>
+      <c r="AI23" s="58"/>
       <c r="AJ23" s="73"/>
     </row>
     <row r="24" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A24" s="179" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="180"/>
-      <c r="C24" s="181"/>
+      <c r="A24" s="140"/>
+      <c r="B24" s="139"/>
+      <c r="C24" s="57"/>
       <c r="D24" s="57"/>
       <c r="E24" s="57"/>
       <c r="F24" s="57"/>
@@ -5659,697 +5674,1305 @@
       <c r="AF24" s="57"/>
       <c r="AG24" s="57"/>
       <c r="AH24" s="57"/>
-      <c r="AI24" s="58">
-        <f>SUM(D24:AH24)</f>
+      <c r="AI24" s="58"/>
+      <c r="AJ24" s="73"/>
+    </row>
+    <row r="25" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+      <c r="A25" s="140"/>
+      <c r="B25" s="139"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="50"/>
+      <c r="L25" s="50"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="50"/>
+      <c r="O25" s="50"/>
+      <c r="P25" s="50"/>
+      <c r="Q25" s="50"/>
+      <c r="R25" s="50"/>
+      <c r="S25" s="50"/>
+      <c r="T25" s="50"/>
+      <c r="U25" s="50"/>
+      <c r="V25" s="50"/>
+      <c r="W25" s="50"/>
+      <c r="X25" s="50"/>
+      <c r="Y25" s="50"/>
+      <c r="Z25" s="50"/>
+      <c r="AA25" s="50"/>
+      <c r="AB25" s="50"/>
+      <c r="AC25" s="50"/>
+      <c r="AD25" s="50"/>
+      <c r="AE25" s="50"/>
+      <c r="AF25" s="57"/>
+      <c r="AG25" s="57"/>
+      <c r="AH25" s="57"/>
+      <c r="AI25" s="58"/>
+      <c r="AJ25" s="73"/>
+    </row>
+    <row r="26" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+      <c r="A26" s="140"/>
+      <c r="B26" s="139"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="50"/>
+      <c r="P26" s="50"/>
+      <c r="Q26" s="50"/>
+      <c r="R26" s="50"/>
+      <c r="S26" s="50"/>
+      <c r="T26" s="50"/>
+      <c r="U26" s="50"/>
+      <c r="V26" s="50"/>
+      <c r="W26" s="50"/>
+      <c r="X26" s="50"/>
+      <c r="Y26" s="50"/>
+      <c r="Z26" s="50"/>
+      <c r="AA26" s="50"/>
+      <c r="AB26" s="50"/>
+      <c r="AC26" s="50"/>
+      <c r="AD26" s="50"/>
+      <c r="AE26" s="50"/>
+      <c r="AF26" s="57"/>
+      <c r="AG26" s="57"/>
+      <c r="AH26" s="57"/>
+      <c r="AI26" s="58"/>
+      <c r="AJ26" s="73"/>
+    </row>
+    <row r="27" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+      <c r="A27" s="140"/>
+      <c r="B27" s="139"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="57"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="50"/>
+      <c r="O27" s="50"/>
+      <c r="P27" s="50"/>
+      <c r="Q27" s="50"/>
+      <c r="R27" s="50"/>
+      <c r="S27" s="50"/>
+      <c r="T27" s="50"/>
+      <c r="U27" s="50"/>
+      <c r="V27" s="50"/>
+      <c r="W27" s="50"/>
+      <c r="X27" s="50"/>
+      <c r="Y27" s="50"/>
+      <c r="Z27" s="50"/>
+      <c r="AA27" s="50"/>
+      <c r="AB27" s="50"/>
+      <c r="AC27" s="50"/>
+      <c r="AD27" s="50"/>
+      <c r="AE27" s="50"/>
+      <c r="AF27" s="57"/>
+      <c r="AG27" s="57"/>
+      <c r="AH27" s="57"/>
+      <c r="AI27" s="58"/>
+      <c r="AJ27" s="73"/>
+    </row>
+    <row r="28" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+      <c r="A28" s="140"/>
+      <c r="B28" s="139"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="50"/>
+      <c r="P28" s="50"/>
+      <c r="Q28" s="50"/>
+      <c r="R28" s="50"/>
+      <c r="S28" s="50"/>
+      <c r="T28" s="50"/>
+      <c r="U28" s="50"/>
+      <c r="V28" s="50"/>
+      <c r="W28" s="50"/>
+      <c r="X28" s="50"/>
+      <c r="Y28" s="50"/>
+      <c r="Z28" s="50"/>
+      <c r="AA28" s="50"/>
+      <c r="AB28" s="50"/>
+      <c r="AC28" s="50"/>
+      <c r="AD28" s="50"/>
+      <c r="AE28" s="50"/>
+      <c r="AF28" s="57"/>
+      <c r="AG28" s="57"/>
+      <c r="AH28" s="57"/>
+      <c r="AI28" s="58"/>
+      <c r="AJ28" s="73"/>
+    </row>
+    <row r="29" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+      <c r="A29" s="140"/>
+      <c r="B29" s="139"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="50"/>
+      <c r="N29" s="50"/>
+      <c r="O29" s="50"/>
+      <c r="P29" s="50"/>
+      <c r="Q29" s="50"/>
+      <c r="R29" s="50"/>
+      <c r="S29" s="50"/>
+      <c r="T29" s="50"/>
+      <c r="U29" s="50"/>
+      <c r="V29" s="50"/>
+      <c r="W29" s="50"/>
+      <c r="X29" s="50"/>
+      <c r="Y29" s="50"/>
+      <c r="Z29" s="50"/>
+      <c r="AA29" s="50"/>
+      <c r="AB29" s="50"/>
+      <c r="AC29" s="50"/>
+      <c r="AD29" s="50"/>
+      <c r="AE29" s="50"/>
+      <c r="AF29" s="57"/>
+      <c r="AG29" s="57"/>
+      <c r="AH29" s="57"/>
+      <c r="AI29" s="58"/>
+      <c r="AJ29" s="73"/>
+    </row>
+    <row r="30" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+      <c r="A30" s="89"/>
+      <c r="B30" s="89"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="50"/>
+      <c r="P30" s="50"/>
+      <c r="Q30" s="50"/>
+      <c r="R30" s="50"/>
+      <c r="S30" s="50"/>
+      <c r="T30" s="50"/>
+      <c r="U30" s="50"/>
+      <c r="V30" s="50"/>
+      <c r="W30" s="50"/>
+      <c r="X30" s="50"/>
+      <c r="Y30" s="50"/>
+      <c r="Z30" s="50"/>
+      <c r="AA30" s="50"/>
+      <c r="AB30" s="50"/>
+      <c r="AC30" s="50"/>
+      <c r="AD30" s="50"/>
+      <c r="AE30" s="50"/>
+      <c r="AF30" s="57"/>
+      <c r="AG30" s="57"/>
+      <c r="AH30" s="57"/>
+      <c r="AI30" s="58"/>
+      <c r="AJ30" s="73"/>
+    </row>
+    <row r="31" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+      <c r="A31" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="59"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="54"/>
+      <c r="H31" s="54"/>
+      <c r="I31" s="54"/>
+      <c r="J31" s="54"/>
+      <c r="K31" s="54"/>
+      <c r="L31" s="54"/>
+      <c r="M31" s="54"/>
+      <c r="N31" s="54"/>
+      <c r="O31" s="54"/>
+      <c r="P31" s="54"/>
+      <c r="Q31" s="54"/>
+      <c r="R31" s="54"/>
+      <c r="S31" s="54"/>
+      <c r="T31" s="54"/>
+      <c r="U31" s="54"/>
+      <c r="V31" s="54"/>
+      <c r="W31" s="54"/>
+      <c r="X31" s="54"/>
+      <c r="Y31" s="54"/>
+      <c r="Z31" s="54"/>
+      <c r="AA31" s="54"/>
+      <c r="AB31" s="54"/>
+      <c r="AC31" s="54"/>
+      <c r="AD31" s="54"/>
+      <c r="AE31" s="54"/>
+      <c r="AF31" s="54"/>
+      <c r="AG31" s="54"/>
+      <c r="AH31" s="54"/>
+      <c r="AI31" s="55"/>
+      <c r="AJ31" s="73"/>
+    </row>
+    <row r="32" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+      <c r="A32" s="67"/>
+      <c r="B32" s="56" t="s">
+        <v>169</v>
+      </c>
+      <c r="C32" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="57">
+        <v>1</v>
+      </c>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="50">
+        <v>1</v>
+      </c>
+      <c r="H32" s="57">
+        <v>1</v>
+      </c>
+      <c r="I32" s="50"/>
+      <c r="J32" s="50"/>
+      <c r="K32" s="50">
+        <v>1</v>
+      </c>
+      <c r="L32" s="50"/>
+      <c r="M32" s="50"/>
+      <c r="N32" s="50">
+        <v>1</v>
+      </c>
+      <c r="O32" s="50">
+        <v>1</v>
+      </c>
+      <c r="P32" s="50"/>
+      <c r="Q32" s="50">
+        <v>1</v>
+      </c>
+      <c r="R32" s="50">
+        <v>1</v>
+      </c>
+      <c r="S32" s="50"/>
+      <c r="T32" s="50"/>
+      <c r="U32" s="50">
+        <v>1</v>
+      </c>
+      <c r="V32" s="50">
+        <v>1</v>
+      </c>
+      <c r="W32" s="50">
+        <v>1</v>
+      </c>
+      <c r="X32" s="50">
+        <v>1</v>
+      </c>
+      <c r="Y32" s="50">
+        <v>1</v>
+      </c>
+      <c r="Z32" s="50"/>
+      <c r="AA32" s="50"/>
+      <c r="AB32" s="50">
+        <v>1</v>
+      </c>
+      <c r="AC32" s="50">
+        <v>1</v>
+      </c>
+      <c r="AD32" s="50">
+        <v>1</v>
+      </c>
+      <c r="AE32" s="50">
+        <v>1</v>
+      </c>
+      <c r="AF32" s="57">
+        <v>1</v>
+      </c>
+      <c r="AG32" s="57"/>
+      <c r="AH32" s="57"/>
+      <c r="AI32" s="58">
+        <f>SUM(D32:AH32)</f>
+        <v>18</v>
+      </c>
+      <c r="AJ32" s="73"/>
+    </row>
+    <row r="33" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+      <c r="A33" s="67"/>
+      <c r="B33" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="C33" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="57"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="50"/>
+      <c r="H33" s="57"/>
+      <c r="I33" s="50"/>
+      <c r="J33" s="50"/>
+      <c r="K33" s="50"/>
+      <c r="L33" s="50"/>
+      <c r="M33" s="50"/>
+      <c r="N33" s="50"/>
+      <c r="O33" s="50"/>
+      <c r="P33" s="50"/>
+      <c r="Q33" s="50"/>
+      <c r="R33" s="50"/>
+      <c r="S33" s="50"/>
+      <c r="T33" s="50"/>
+      <c r="U33" s="50"/>
+      <c r="V33" s="50"/>
+      <c r="W33" s="50"/>
+      <c r="X33" s="50"/>
+      <c r="Y33" s="50"/>
+      <c r="Z33" s="50"/>
+      <c r="AA33" s="50"/>
+      <c r="AB33" s="50"/>
+      <c r="AC33" s="50"/>
+      <c r="AD33" s="50"/>
+      <c r="AE33" s="50"/>
+      <c r="AF33" s="57"/>
+      <c r="AG33" s="57"/>
+      <c r="AH33" s="57"/>
+      <c r="AI33" s="58">
+        <f>SUM(D33:AH33)</f>
         <v>0</v>
       </c>
-      <c r="AJ24" s="73"/>
-    </row>
-    <row r="25" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A25" s="176" t="s">
+      <c r="AJ33" s="73"/>
+    </row>
+    <row r="34" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+      <c r="A34" s="67"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="50"/>
+      <c r="J34" s="50"/>
+      <c r="K34" s="50"/>
+      <c r="L34" s="50"/>
+      <c r="M34" s="50"/>
+      <c r="N34" s="50"/>
+      <c r="O34" s="50"/>
+      <c r="P34" s="50"/>
+      <c r="Q34" s="50"/>
+      <c r="R34" s="50"/>
+      <c r="S34" s="50"/>
+      <c r="T34" s="50"/>
+      <c r="U34" s="50"/>
+      <c r="V34" s="50"/>
+      <c r="W34" s="50"/>
+      <c r="X34" s="50"/>
+      <c r="Y34" s="50"/>
+      <c r="Z34" s="50"/>
+      <c r="AA34" s="50"/>
+      <c r="AB34" s="50"/>
+      <c r="AC34" s="50"/>
+      <c r="AD34" s="50"/>
+      <c r="AE34" s="50"/>
+      <c r="AF34" s="57"/>
+      <c r="AG34" s="57"/>
+      <c r="AH34" s="57"/>
+      <c r="AI34" s="58">
+        <f>SUM(D34:AH34)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ34" s="73"/>
+    </row>
+    <row r="35" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="68"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="61"/>
+      <c r="I35" s="61"/>
+      <c r="J35" s="61"/>
+      <c r="K35" s="61"/>
+      <c r="L35" s="61"/>
+      <c r="M35" s="61"/>
+      <c r="N35" s="61"/>
+      <c r="O35" s="61"/>
+      <c r="P35" s="61"/>
+      <c r="Q35" s="61"/>
+      <c r="R35" s="61"/>
+      <c r="S35" s="61"/>
+      <c r="T35" s="61"/>
+      <c r="U35" s="61"/>
+      <c r="V35" s="61"/>
+      <c r="W35" s="61"/>
+      <c r="X35" s="61"/>
+      <c r="Y35" s="61"/>
+      <c r="Z35" s="61"/>
+      <c r="AA35" s="61"/>
+      <c r="AB35" s="61"/>
+      <c r="AC35" s="61"/>
+      <c r="AD35" s="61"/>
+      <c r="AE35" s="61"/>
+      <c r="AF35" s="61"/>
+      <c r="AG35" s="205"/>
+      <c r="AH35" s="62"/>
+      <c r="AI35" s="62"/>
+      <c r="AJ35" s="73"/>
+    </row>
+    <row r="36" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+      <c r="A36" s="178" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="179"/>
+      <c r="C36" s="180"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="50"/>
+      <c r="K36" s="50"/>
+      <c r="L36" s="50"/>
+      <c r="M36" s="50"/>
+      <c r="N36" s="50"/>
+      <c r="O36" s="50"/>
+      <c r="P36" s="50"/>
+      <c r="Q36" s="50"/>
+      <c r="R36" s="50"/>
+      <c r="S36" s="50"/>
+      <c r="T36" s="50"/>
+      <c r="U36" s="50"/>
+      <c r="V36" s="50"/>
+      <c r="W36" s="50"/>
+      <c r="X36" s="50"/>
+      <c r="Y36" s="50"/>
+      <c r="Z36" s="50"/>
+      <c r="AA36" s="50"/>
+      <c r="AB36" s="50"/>
+      <c r="AC36" s="50"/>
+      <c r="AD36" s="50"/>
+      <c r="AE36" s="50"/>
+      <c r="AF36" s="57"/>
+      <c r="AG36" s="57"/>
+      <c r="AH36" s="57"/>
+      <c r="AI36" s="58">
+        <f>SUM(D36:AH36)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ36" s="73"/>
+    </row>
+    <row r="37" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+      <c r="A37" s="178" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="179"/>
+      <c r="C37" s="180"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="50"/>
+      <c r="K37" s="50"/>
+      <c r="L37" s="50"/>
+      <c r="M37" s="50"/>
+      <c r="N37" s="50"/>
+      <c r="O37" s="50"/>
+      <c r="P37" s="50"/>
+      <c r="Q37" s="50"/>
+      <c r="R37" s="50"/>
+      <c r="S37" s="50"/>
+      <c r="T37" s="50"/>
+      <c r="U37" s="50"/>
+      <c r="V37" s="50"/>
+      <c r="W37" s="50"/>
+      <c r="X37" s="50"/>
+      <c r="Y37" s="50"/>
+      <c r="Z37" s="50"/>
+      <c r="AA37" s="50"/>
+      <c r="AB37" s="50"/>
+      <c r="AC37" s="50"/>
+      <c r="AD37" s="50"/>
+      <c r="AE37" s="50"/>
+      <c r="AF37" s="57"/>
+      <c r="AG37" s="57"/>
+      <c r="AH37" s="57"/>
+      <c r="AI37" s="58">
+        <f>SUM(D37:AH37)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ37" s="73"/>
+    </row>
+    <row r="38" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+      <c r="A38" s="181" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="182"/>
+      <c r="C38" s="183"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="50">
+        <v>8</v>
+      </c>
+      <c r="J38" s="50">
+        <v>8</v>
+      </c>
+      <c r="K38" s="50"/>
+      <c r="L38" s="50"/>
+      <c r="M38" s="50"/>
+      <c r="N38" s="50"/>
+      <c r="O38" s="50"/>
+      <c r="P38" s="50">
+        <v>8</v>
+      </c>
+      <c r="Q38" s="50"/>
+      <c r="R38" s="50"/>
+      <c r="S38" s="50"/>
+      <c r="T38" s="50"/>
+      <c r="U38" s="50"/>
+      <c r="V38" s="50"/>
+      <c r="W38" s="50"/>
+      <c r="X38" s="50"/>
+      <c r="Y38" s="50"/>
+      <c r="Z38" s="50"/>
+      <c r="AA38" s="50"/>
+      <c r="AB38" s="50"/>
+      <c r="AC38" s="50"/>
+      <c r="AD38" s="50"/>
+      <c r="AE38" s="50"/>
+      <c r="AF38" s="57"/>
+      <c r="AG38" s="57"/>
+      <c r="AH38" s="57"/>
+      <c r="AI38" s="58">
+        <f>SUM(D38:AH38)</f>
+        <v>24</v>
+      </c>
+      <c r="AJ38" s="73"/>
+    </row>
+    <row r="39" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+      <c r="A39" s="178" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="177"/>
-      <c r="C25" s="178"/>
-      <c r="D25" s="57">
-        <f t="shared" ref="D25:AB25" si="1">SUM(D11:D20)</f>
+      <c r="B39" s="179"/>
+      <c r="C39" s="180"/>
+      <c r="D39" s="57">
+        <f t="shared" ref="D39:AC39" si="2">SUM(D11:D34)</f>
+        <v>8</v>
+      </c>
+      <c r="E39" s="57">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E25" s="57">
-        <f t="shared" si="1"/>
+      <c r="F39" s="57">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F25" s="57">
-        <f t="shared" si="1"/>
+      <c r="G39" s="57">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="H39" s="57">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="I39" s="50">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G25" s="57">
-        <f t="shared" si="1"/>
+      <c r="J39" s="50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K39" s="50">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="H25" s="57">
-        <f t="shared" si="1"/>
+      <c r="L39" s="50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M39" s="50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N39" s="50">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="I25" s="50">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="J25" s="50">
-        <f t="shared" si="1"/>
+      <c r="O39" s="50">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="P39" s="50">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K25" s="50">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="L25" s="50">
-        <f t="shared" si="1"/>
+      <c r="Q39" s="50">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="R39" s="50">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="S39" s="50">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M25" s="50">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="N25" s="50">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="O25" s="50">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="P25" s="50">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="Q25" s="50">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="R25" s="50">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="S25" s="50">
-        <f t="shared" si="1"/>
+      <c r="T39" s="50">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T25" s="50">
-        <f t="shared" si="1"/>
+      <c r="U39" s="50">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V39" s="50">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="W39" s="50">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="X39" s="50">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Y39" s="50">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Z39" s="50">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U25" s="50">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="V25" s="50">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="W25" s="50">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="X25" s="50">
-        <f t="shared" si="1"/>
+      <c r="AA39" s="50">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y25" s="50">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="Z25" s="50">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="AA25" s="50">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="AB25" s="50">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="AC25" s="50">
-        <v>8</v>
-      </c>
-      <c r="AD25" s="50">
-        <f>SUM(AD11:AD20)</f>
-        <v>8</v>
-      </c>
-      <c r="AE25" s="50">
-        <f>SUM(AE11:AE20)</f>
+      <c r="AB39" s="50">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AC39" s="50">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AD39" s="50">
+        <f>SUM(AD11:AD34)</f>
+        <v>1</v>
+      </c>
+      <c r="AE39" s="50">
+        <f>SUM(AE11:AE34)</f>
+        <v>1</v>
+      </c>
+      <c r="AF39" s="57">
+        <f>SUM(AF11:AF34)</f>
+        <v>1</v>
+      </c>
+      <c r="AG39" s="57">
         <v>0</v>
       </c>
-      <c r="AF25" s="57">
-        <f>SUM(AF11:AF20)</f>
+      <c r="AH39" s="57">
+        <f>SUM(AH11:AH34)</f>
         <v>0</v>
       </c>
-      <c r="AG25" s="57">
-        <f>SUM(AG11:AG20)</f>
-        <v>8</v>
-      </c>
-      <c r="AH25" s="57">
-        <f>SUM(AH11:AH20)</f>
-        <v>0</v>
-      </c>
-      <c r="AI25" s="58">
-        <f>SUM(D25:AH25)</f>
-        <v>163</v>
-      </c>
-      <c r="AJ25" s="73"/>
-    </row>
-    <row r="26" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="27" spans="1:36" s="93" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="91"/>
-      <c r="B27" s="92" t="s">
+      <c r="AI39" s="58">
+        <f>SUM(D39:AH39)</f>
+        <v>64</v>
+      </c>
+      <c r="AJ39" s="73"/>
+    </row>
+    <row r="40" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="41" spans="1:36" s="93" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="91"/>
+      <c r="B41" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="143"/>
-      <c r="F27" s="143"/>
-      <c r="G27" s="143"/>
-      <c r="H27" s="143"/>
-      <c r="I27" s="143"/>
-      <c r="J27" s="143"/>
-      <c r="S27" s="196" t="s">
+      <c r="D41" s="4"/>
+      <c r="E41" s="145"/>
+      <c r="F41" s="145"/>
+      <c r="G41" s="145"/>
+      <c r="H41" s="145"/>
+      <c r="I41" s="145"/>
+      <c r="J41" s="145"/>
+      <c r="S41" s="201" t="s">
         <v>43</v>
       </c>
-      <c r="T27" s="197"/>
-      <c r="U27" s="197"/>
-      <c r="V27" s="197"/>
-      <c r="W27" s="197"/>
-      <c r="X27" s="197"/>
-      <c r="Y27" s="197"/>
-      <c r="Z27" s="197"/>
-      <c r="AA27" s="198"/>
-      <c r="AC27" s="182" t="s">
+      <c r="T41" s="202"/>
+      <c r="U41" s="202"/>
+      <c r="V41" s="202"/>
+      <c r="W41" s="202"/>
+      <c r="X41" s="202"/>
+      <c r="Y41" s="202"/>
+      <c r="Z41" s="202"/>
+      <c r="AA41" s="203"/>
+      <c r="AC41" s="187" t="s">
         <v>44</v>
       </c>
-      <c r="AD27" s="183"/>
-      <c r="AE27" s="183"/>
-      <c r="AF27" s="183"/>
-      <c r="AG27" s="183"/>
-      <c r="AH27" s="183"/>
-      <c r="AI27" s="183"/>
-      <c r="AJ27" s="184"/>
-    </row>
-    <row r="28" spans="1:36" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="69"/>
-      <c r="B28" s="49" t="s">
+      <c r="AD41" s="188"/>
+      <c r="AE41" s="188"/>
+      <c r="AF41" s="188"/>
+      <c r="AG41" s="188"/>
+      <c r="AH41" s="188"/>
+      <c r="AI41" s="188"/>
+      <c r="AJ41" s="189"/>
+    </row>
+    <row r="42" spans="1:36" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="69"/>
+      <c r="B42" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="143"/>
-      <c r="F28" s="143"/>
-      <c r="G28" s="143"/>
-      <c r="H28" s="143"/>
-      <c r="I28" s="143"/>
-      <c r="J28" s="143"/>
-      <c r="S28" s="185" t="s">
+      <c r="E42" s="145"/>
+      <c r="F42" s="145"/>
+      <c r="G42" s="145"/>
+      <c r="H42" s="145"/>
+      <c r="I42" s="145"/>
+      <c r="J42" s="145"/>
+      <c r="S42" s="190" t="s">
         <v>46</v>
       </c>
-      <c r="T28" s="186"/>
-      <c r="U28" s="187" t="s">
+      <c r="T42" s="191"/>
+      <c r="U42" s="192" t="s">
         <v>47</v>
       </c>
-      <c r="V28" s="187"/>
-      <c r="W28" s="187"/>
-      <c r="X28" s="187"/>
-      <c r="Y28" s="187"/>
-      <c r="Z28" s="187"/>
-      <c r="AA28" s="188"/>
-      <c r="AC28" s="159" t="s">
+      <c r="V42" s="192"/>
+      <c r="W42" s="192"/>
+      <c r="X42" s="192"/>
+      <c r="Y42" s="192"/>
+      <c r="Z42" s="192"/>
+      <c r="AA42" s="193"/>
+      <c r="AC42" s="161" t="s">
         <v>48</v>
       </c>
-      <c r="AD28" s="145"/>
-      <c r="AE28" s="145"/>
-      <c r="AF28" s="145"/>
-      <c r="AG28" s="145"/>
-      <c r="AH28" s="145"/>
-      <c r="AI28" s="145"/>
-      <c r="AJ28" s="146"/>
-    </row>
-    <row r="29" spans="1:36" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="70"/>
-      <c r="B29" s="49" t="s">
+      <c r="AD42" s="147"/>
+      <c r="AE42" s="147"/>
+      <c r="AF42" s="147"/>
+      <c r="AG42" s="147"/>
+      <c r="AH42" s="147"/>
+      <c r="AI42" s="147"/>
+      <c r="AJ42" s="148"/>
+    </row>
+    <row r="43" spans="1:36" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="70"/>
+      <c r="B43" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="E29" s="143"/>
-      <c r="F29" s="143"/>
-      <c r="G29" s="143"/>
-      <c r="H29" s="143"/>
-      <c r="I29" s="143"/>
-      <c r="J29" s="143"/>
-      <c r="S29" s="185"/>
-      <c r="T29" s="186"/>
-      <c r="U29" s="187"/>
-      <c r="V29" s="187"/>
-      <c r="W29" s="187"/>
-      <c r="X29" s="187"/>
-      <c r="Y29" s="187"/>
-      <c r="Z29" s="187"/>
-      <c r="AA29" s="188"/>
-      <c r="AC29" s="160"/>
-      <c r="AD29" s="148"/>
-      <c r="AE29" s="148"/>
-      <c r="AF29" s="148"/>
-      <c r="AG29" s="148"/>
-      <c r="AH29" s="148"/>
-      <c r="AI29" s="148"/>
-      <c r="AJ29" s="149"/>
-    </row>
-    <row r="30" spans="1:36" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="71"/>
-      <c r="B30" s="49" t="s">
+      <c r="E43" s="145"/>
+      <c r="F43" s="145"/>
+      <c r="G43" s="145"/>
+      <c r="H43" s="145"/>
+      <c r="I43" s="145"/>
+      <c r="J43" s="145"/>
+      <c r="S43" s="190"/>
+      <c r="T43" s="191"/>
+      <c r="U43" s="192"/>
+      <c r="V43" s="192"/>
+      <c r="W43" s="192"/>
+      <c r="X43" s="192"/>
+      <c r="Y43" s="192"/>
+      <c r="Z43" s="192"/>
+      <c r="AA43" s="193"/>
+      <c r="AC43" s="162"/>
+      <c r="AD43" s="150"/>
+      <c r="AE43" s="150"/>
+      <c r="AF43" s="150"/>
+      <c r="AG43" s="150"/>
+      <c r="AH43" s="150"/>
+      <c r="AI43" s="150"/>
+      <c r="AJ43" s="151"/>
+    </row>
+    <row r="44" spans="1:36" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="71"/>
+      <c r="B44" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="E30" s="143"/>
-      <c r="F30" s="143"/>
-      <c r="G30" s="143"/>
-      <c r="H30" s="143"/>
-      <c r="I30" s="143"/>
-      <c r="J30" s="143"/>
-      <c r="S30" s="185"/>
-      <c r="T30" s="186"/>
-      <c r="U30" s="187"/>
-      <c r="V30" s="187"/>
-      <c r="W30" s="187"/>
-      <c r="X30" s="187"/>
-      <c r="Y30" s="187"/>
-      <c r="Z30" s="187"/>
-      <c r="AA30" s="188"/>
-      <c r="AC30" s="160"/>
-      <c r="AD30" s="148"/>
-      <c r="AE30" s="148"/>
-      <c r="AF30" s="148"/>
-      <c r="AG30" s="148"/>
-      <c r="AH30" s="148"/>
-      <c r="AI30" s="148"/>
-      <c r="AJ30" s="149"/>
-    </row>
-    <row r="31" spans="1:36" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="S31" s="185"/>
-      <c r="T31" s="186"/>
-      <c r="U31" s="187"/>
-      <c r="V31" s="187"/>
-      <c r="W31" s="187"/>
-      <c r="X31" s="187"/>
-      <c r="Y31" s="187"/>
-      <c r="Z31" s="187"/>
-      <c r="AA31" s="188"/>
-      <c r="AC31" s="160"/>
-      <c r="AD31" s="148"/>
-      <c r="AE31" s="148"/>
-      <c r="AF31" s="148"/>
-      <c r="AG31" s="148"/>
-      <c r="AH31" s="148"/>
-      <c r="AI31" s="148"/>
-      <c r="AJ31" s="149"/>
-    </row>
-    <row r="32" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A32" s="72" t="s">
+      <c r="E44" s="145"/>
+      <c r="F44" s="145"/>
+      <c r="G44" s="145"/>
+      <c r="H44" s="145"/>
+      <c r="I44" s="145"/>
+      <c r="J44" s="145"/>
+      <c r="S44" s="190"/>
+      <c r="T44" s="191"/>
+      <c r="U44" s="192"/>
+      <c r="V44" s="192"/>
+      <c r="W44" s="192"/>
+      <c r="X44" s="192"/>
+      <c r="Y44" s="192"/>
+      <c r="Z44" s="192"/>
+      <c r="AA44" s="193"/>
+      <c r="AC44" s="162"/>
+      <c r="AD44" s="150"/>
+      <c r="AE44" s="150"/>
+      <c r="AF44" s="150"/>
+      <c r="AG44" s="150"/>
+      <c r="AH44" s="150"/>
+      <c r="AI44" s="150"/>
+      <c r="AJ44" s="151"/>
+    </row>
+    <row r="45" spans="1:36" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="S45" s="190"/>
+      <c r="T45" s="191"/>
+      <c r="U45" s="192"/>
+      <c r="V45" s="192"/>
+      <c r="W45" s="192"/>
+      <c r="X45" s="192"/>
+      <c r="Y45" s="192"/>
+      <c r="Z45" s="192"/>
+      <c r="AA45" s="193"/>
+      <c r="AC45" s="162"/>
+      <c r="AD45" s="150"/>
+      <c r="AE45" s="150"/>
+      <c r="AF45" s="150"/>
+      <c r="AG45" s="150"/>
+      <c r="AH45" s="150"/>
+      <c r="AI45" s="150"/>
+      <c r="AJ45" s="151"/>
+    </row>
+    <row r="46" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A46" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="46"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="44"/>
-      <c r="S32" s="185"/>
-      <c r="T32" s="186"/>
-      <c r="U32" s="187"/>
-      <c r="V32" s="187"/>
-      <c r="W32" s="187"/>
-      <c r="X32" s="187"/>
-      <c r="Y32" s="187"/>
-      <c r="Z32" s="187"/>
-      <c r="AA32" s="188"/>
-      <c r="AC32" s="189"/>
-      <c r="AD32" s="190"/>
-      <c r="AE32" s="190"/>
-      <c r="AF32" s="190"/>
-      <c r="AG32" s="190"/>
-      <c r="AH32" s="190"/>
-      <c r="AI32" s="190"/>
-      <c r="AJ32" s="191"/>
-    </row>
-    <row r="33" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A33" s="140" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" s="140"/>
-      <c r="C33" s="63">
-        <f>COUNTIF(D24:AH24,"=8")</f>
-        <v>0</v>
-      </c>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="44"/>
-      <c r="S33" s="185" t="s">
-        <v>53</v>
-      </c>
-      <c r="T33" s="186"/>
-      <c r="U33" s="187" t="s">
-        <v>54</v>
-      </c>
-      <c r="V33" s="187"/>
-      <c r="W33" s="187"/>
-      <c r="X33" s="187"/>
-      <c r="Y33" s="187"/>
-      <c r="Z33" s="187"/>
-      <c r="AA33" s="188"/>
-      <c r="AC33" s="160" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD33" s="148"/>
-      <c r="AE33" s="148"/>
-      <c r="AF33" s="148"/>
-      <c r="AG33" s="148"/>
-      <c r="AH33" s="148"/>
-      <c r="AI33" s="148"/>
-      <c r="AJ33" s="149"/>
-    </row>
-    <row r="34" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A34" s="63" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="47"/>
-      <c r="C34" s="64">
-        <f>NETWORKDAYS(B2,B3)-C33</f>
-        <v>21</v>
-      </c>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="44"/>
-      <c r="H34" s="44"/>
-      <c r="S34" s="185"/>
-      <c r="T34" s="186"/>
-      <c r="U34" s="187"/>
-      <c r="V34" s="187"/>
-      <c r="W34" s="187"/>
-      <c r="X34" s="187"/>
-      <c r="Y34" s="187"/>
-      <c r="Z34" s="187"/>
-      <c r="AA34" s="188"/>
-      <c r="AC34" s="160"/>
-      <c r="AD34" s="148"/>
-      <c r="AE34" s="148"/>
-      <c r="AF34" s="148"/>
-      <c r="AG34" s="148"/>
-      <c r="AH34" s="148"/>
-      <c r="AI34" s="148"/>
-      <c r="AJ34" s="149"/>
-    </row>
-    <row r="35" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A35" s="63" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" s="47"/>
-      <c r="C35" s="63">
-        <f>AI23/8</f>
-        <v>0</v>
-      </c>
-      <c r="D35" s="44"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="44"/>
-      <c r="H35" s="44"/>
-      <c r="S35" s="185"/>
-      <c r="T35" s="186"/>
-      <c r="U35" s="187"/>
-      <c r="V35" s="187"/>
-      <c r="W35" s="187"/>
-      <c r="X35" s="187"/>
-      <c r="Y35" s="187"/>
-      <c r="Z35" s="187"/>
-      <c r="AA35" s="188"/>
-      <c r="AC35" s="160"/>
-      <c r="AD35" s="148"/>
-      <c r="AE35" s="148"/>
-      <c r="AF35" s="148"/>
-      <c r="AG35" s="148"/>
-      <c r="AH35" s="148"/>
-      <c r="AI35" s="148"/>
-      <c r="AJ35" s="149"/>
-    </row>
-    <row r="36" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A36" s="63" t="s">
-        <v>58</v>
-      </c>
-      <c r="B36" s="47"/>
-      <c r="C36" s="63">
-        <f>AI22/8</f>
-        <v>0</v>
-      </c>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="44"/>
-      <c r="S36" s="185"/>
-      <c r="T36" s="186"/>
-      <c r="U36" s="187"/>
-      <c r="V36" s="187"/>
-      <c r="W36" s="187"/>
-      <c r="X36" s="187"/>
-      <c r="Y36" s="187"/>
-      <c r="Z36" s="187"/>
-      <c r="AA36" s="188"/>
-      <c r="AC36" s="160"/>
-      <c r="AD36" s="148"/>
-      <c r="AE36" s="148"/>
-      <c r="AF36" s="148"/>
-      <c r="AG36" s="148"/>
-      <c r="AH36" s="148"/>
-      <c r="AI36" s="148"/>
-      <c r="AJ36" s="149"/>
-    </row>
-    <row r="37" spans="1:36" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="174" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" s="174"/>
-      <c r="C37" s="63">
-        <f>COUNTIF(D25:AH25,"&gt;0")</f>
-        <v>20</v>
-      </c>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="44"/>
-      <c r="H37" s="44"/>
-      <c r="S37" s="192"/>
-      <c r="T37" s="193"/>
-      <c r="U37" s="194"/>
-      <c r="V37" s="194"/>
-      <c r="W37" s="194"/>
-      <c r="X37" s="194"/>
-      <c r="Y37" s="194"/>
-      <c r="Z37" s="194"/>
-      <c r="AA37" s="195"/>
-      <c r="AC37" s="161"/>
-      <c r="AD37" s="151"/>
-      <c r="AE37" s="151"/>
-      <c r="AF37" s="151"/>
-      <c r="AG37" s="151"/>
-      <c r="AH37" s="151"/>
-      <c r="AI37" s="151"/>
-      <c r="AJ37" s="152"/>
-    </row>
-    <row r="38" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A38" s="63" t="s">
-        <v>60</v>
-      </c>
-      <c r="B38" s="47"/>
-      <c r="C38" s="65">
-        <f>C37/(C37+C35+C36)</f>
-        <v>1</v>
-      </c>
-      <c r="D38" s="44"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="44"/>
-      <c r="H38" s="44"/>
-    </row>
-    <row r="39" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A39" s="63"/>
-      <c r="B39" s="47"/>
-      <c r="C39" s="63"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="44"/>
-      <c r="H39" s="44"/>
-    </row>
-    <row r="40" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A40" s="72" t="s">
-        <v>61</v>
-      </c>
-      <c r="B40" s="46"/>
-      <c r="C40" s="63"/>
-      <c r="D40" s="44"/>
-      <c r="E40" s="44"/>
-      <c r="F40" s="44"/>
-      <c r="G40" s="44"/>
-      <c r="H40" s="44"/>
-    </row>
-    <row r="41" spans="1:36" ht="35.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="174" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41" s="174"/>
-      <c r="C41" s="63">
-        <f>AI25</f>
-        <v>163</v>
-      </c>
-      <c r="D41" s="44"/>
-      <c r="E41" s="44"/>
-      <c r="F41" s="44"/>
-      <c r="G41" s="44"/>
-      <c r="H41" s="44"/>
-    </row>
-    <row r="42" spans="1:36" ht="38.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="174" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42" s="174"/>
-      <c r="C42" s="63">
-        <v>39</v>
-      </c>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44"/>
-      <c r="F42" s="44"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="44"/>
-    </row>
-    <row r="43" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A43" s="63" t="s">
-        <v>64</v>
-      </c>
-      <c r="B43" s="48"/>
-      <c r="C43" s="63">
-        <f>SUMIFS($AI$12:$AI$20, $C$12:$C$20, "Morning")</f>
-        <v>25</v>
-      </c>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="44"/>
-    </row>
-    <row r="44" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A44" s="63" t="s">
-        <v>65</v>
-      </c>
-      <c r="B44" s="48"/>
-      <c r="C44" s="63">
-        <f>SUMIFS($AI$12:$AI$20, $C$12:$C$20, "Afternoon")</f>
-        <v>7</v>
-      </c>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="44"/>
-    </row>
-    <row r="45" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A45" s="63" t="s">
-        <v>66</v>
-      </c>
-      <c r="B45" s="48"/>
-      <c r="C45" s="63">
-        <f>SUMIFS($AI$12:$AI$20, $C$12:$C$20, "Night")</f>
-        <v>18</v>
-      </c>
-      <c r="D45" s="44"/>
-      <c r="E45" s="44"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="44"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="44"/>
-    </row>
-    <row r="46" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A46" s="63"/>
-      <c r="B46" s="47"/>
+      <c r="B46" s="46"/>
       <c r="C46" s="63"/>
       <c r="D46" s="44"/>
       <c r="E46" s="44"/>
       <c r="F46" s="44"/>
       <c r="G46" s="44"/>
       <c r="H46" s="44"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="S46" s="190"/>
+      <c r="T46" s="191"/>
+      <c r="U46" s="192"/>
+      <c r="V46" s="192"/>
+      <c r="W46" s="192"/>
+      <c r="X46" s="192"/>
+      <c r="Y46" s="192"/>
+      <c r="Z46" s="192"/>
+      <c r="AA46" s="193"/>
+      <c r="AC46" s="194"/>
+      <c r="AD46" s="195"/>
+      <c r="AE46" s="195"/>
+      <c r="AF46" s="195"/>
+      <c r="AG46" s="195"/>
+      <c r="AH46" s="195"/>
+      <c r="AI46" s="195"/>
+      <c r="AJ46" s="196"/>
     </row>
     <row r="47" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A47" s="72" t="s">
-        <v>67</v>
-      </c>
-      <c r="B47" s="46"/>
-      <c r="C47" s="63"/>
+      <c r="A47" s="142" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" s="142"/>
+      <c r="C47" s="63">
+        <f>COUNTIF(D38:AH38,"=8")</f>
+        <v>3</v>
+      </c>
       <c r="D47" s="44"/>
       <c r="E47" s="44"/>
       <c r="F47" s="44"/>
       <c r="G47" s="44"/>
       <c r="H47" s="44"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
+      <c r="S47" s="190" t="s">
+        <v>53</v>
+      </c>
+      <c r="T47" s="191"/>
+      <c r="U47" s="192" t="s">
+        <v>170</v>
+      </c>
+      <c r="V47" s="192"/>
+      <c r="W47" s="192"/>
+      <c r="X47" s="192"/>
+      <c r="Y47" s="192"/>
+      <c r="Z47" s="192"/>
+      <c r="AA47" s="193"/>
+      <c r="AC47" s="162" t="s">
+        <v>183</v>
+      </c>
+      <c r="AD47" s="150"/>
+      <c r="AE47" s="150"/>
+      <c r="AF47" s="150"/>
+      <c r="AG47" s="150"/>
+      <c r="AH47" s="150"/>
+      <c r="AI47" s="150"/>
+      <c r="AJ47" s="151"/>
     </row>
     <row r="48" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A48" s="63" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B48" s="47"/>
-      <c r="C48" s="63"/>
+      <c r="C48" s="64">
+        <f>NETWORKDAYS(B2,B3)-C47</f>
+        <v>18</v>
+      </c>
       <c r="D48" s="44"/>
       <c r="E48" s="44"/>
       <c r="F48" s="44"/>
       <c r="G48" s="44"/>
       <c r="H48" s="44"/>
-      <c r="I48" s="44"/>
-      <c r="J48" s="44"/>
-    </row>
-    <row r="49" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="S48" s="190"/>
+      <c r="T48" s="191"/>
+      <c r="U48" s="192"/>
+      <c r="V48" s="192"/>
+      <c r="W48" s="192"/>
+      <c r="X48" s="192"/>
+      <c r="Y48" s="192"/>
+      <c r="Z48" s="192"/>
+      <c r="AA48" s="193"/>
+      <c r="AC48" s="162"/>
+      <c r="AD48" s="150"/>
+      <c r="AE48" s="150"/>
+      <c r="AF48" s="150"/>
+      <c r="AG48" s="150"/>
+      <c r="AH48" s="150"/>
+      <c r="AI48" s="150"/>
+      <c r="AJ48" s="151"/>
+    </row>
+    <row r="49" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A49" s="63" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B49" s="47"/>
-      <c r="C49" s="63"/>
+      <c r="C49" s="63">
+        <f>AI37/8</f>
+        <v>0</v>
+      </c>
       <c r="D49" s="44"/>
       <c r="E49" s="44"/>
       <c r="F49" s="44"/>
       <c r="G49" s="44"/>
       <c r="H49" s="44"/>
-      <c r="I49" s="44"/>
-      <c r="J49" s="44"/>
-    </row>
-    <row r="50" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A50" s="63"/>
+      <c r="S49" s="190"/>
+      <c r="T49" s="191"/>
+      <c r="U49" s="192"/>
+      <c r="V49" s="192"/>
+      <c r="W49" s="192"/>
+      <c r="X49" s="192"/>
+      <c r="Y49" s="192"/>
+      <c r="Z49" s="192"/>
+      <c r="AA49" s="193"/>
+      <c r="AC49" s="162"/>
+      <c r="AD49" s="150"/>
+      <c r="AE49" s="150"/>
+      <c r="AF49" s="150"/>
+      <c r="AG49" s="150"/>
+      <c r="AH49" s="150"/>
+      <c r="AI49" s="150"/>
+      <c r="AJ49" s="151"/>
+    </row>
+    <row r="50" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A50" s="63" t="s">
+        <v>58</v>
+      </c>
       <c r="B50" s="47"/>
-      <c r="C50" s="63"/>
+      <c r="C50" s="63">
+        <f>AI36/8</f>
+        <v>0</v>
+      </c>
       <c r="D50" s="44"/>
       <c r="E50" s="44"/>
       <c r="F50" s="44"/>
       <c r="G50" s="44"/>
       <c r="H50" s="44"/>
-      <c r="I50" s="44"/>
-      <c r="J50" s="44"/>
-    </row>
-    <row r="52" spans="1:10" ht="155.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="53" spans="1:10" ht="169" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="S50" s="190"/>
+      <c r="T50" s="191"/>
+      <c r="U50" s="192"/>
+      <c r="V50" s="192"/>
+      <c r="W50" s="192"/>
+      <c r="X50" s="192"/>
+      <c r="Y50" s="192"/>
+      <c r="Z50" s="192"/>
+      <c r="AA50" s="193"/>
+      <c r="AC50" s="162"/>
+      <c r="AD50" s="150"/>
+      <c r="AE50" s="150"/>
+      <c r="AF50" s="150"/>
+      <c r="AG50" s="150"/>
+      <c r="AH50" s="150"/>
+      <c r="AI50" s="150"/>
+      <c r="AJ50" s="151"/>
+    </row>
+    <row r="51" spans="1:36" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A51" s="176" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="176"/>
+      <c r="C51" s="63">
+        <f>COUNTIF(D39:AH39,"&gt;0")</f>
+        <v>18</v>
+      </c>
+      <c r="D51" s="44"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
+      <c r="G51" s="44"/>
+      <c r="H51" s="44"/>
+      <c r="S51" s="197"/>
+      <c r="T51" s="198"/>
+      <c r="U51" s="199"/>
+      <c r="V51" s="199"/>
+      <c r="W51" s="199"/>
+      <c r="X51" s="199"/>
+      <c r="Y51" s="199"/>
+      <c r="Z51" s="199"/>
+      <c r="AA51" s="200"/>
+      <c r="AC51" s="163"/>
+      <c r="AD51" s="153"/>
+      <c r="AE51" s="153"/>
+      <c r="AF51" s="153"/>
+      <c r="AG51" s="153"/>
+      <c r="AH51" s="153"/>
+      <c r="AI51" s="153"/>
+      <c r="AJ51" s="154"/>
+    </row>
+    <row r="52" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A52" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" s="47"/>
+      <c r="C52" s="65">
+        <f>C51/(C51+C49+C50)</f>
+        <v>1</v>
+      </c>
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="44"/>
+      <c r="H52" s="44"/>
+    </row>
+    <row r="53" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A53" s="63"/>
+      <c r="B53" s="47"/>
+      <c r="C53" s="63"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="44"/>
+      <c r="H53" s="44"/>
+    </row>
+    <row r="54" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A54" s="72" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" s="46"/>
+      <c r="C54" s="63"/>
+      <c r="D54" s="44"/>
+      <c r="E54" s="44"/>
+      <c r="F54" s="44"/>
+      <c r="G54" s="44"/>
+      <c r="H54" s="44"/>
+    </row>
+    <row r="55" spans="1:36" ht="35.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A55" s="176" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" s="176"/>
+      <c r="C55" s="63">
+        <f>AI39</f>
+        <v>64</v>
+      </c>
+      <c r="D55" s="44"/>
+      <c r="E55" s="44"/>
+      <c r="F55" s="44"/>
+      <c r="G55" s="44"/>
+      <c r="H55" s="44"/>
+    </row>
+    <row r="56" spans="1:36" ht="38.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="176" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56" s="176"/>
+      <c r="C56" s="63">
+        <v>39</v>
+      </c>
+      <c r="D56" s="44"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="44"/>
+      <c r="H56" s="44"/>
+    </row>
+    <row r="57" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A57" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="B57" s="48"/>
+      <c r="C57" s="63">
+        <f>SUMIFS($AI$12:$AI$34, $C$12:$C$34, "Morning")</f>
+        <v>18</v>
+      </c>
+      <c r="D57" s="44"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
+      <c r="G57" s="44"/>
+      <c r="H57" s="44"/>
+    </row>
+    <row r="58" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A58" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" s="48"/>
+      <c r="C58" s="63">
+        <f>SUMIFS($AI$12:$AI$34, $C$12:$C$34, "Afternoon")</f>
+        <v>0</v>
+      </c>
+      <c r="D58" s="44"/>
+      <c r="E58" s="44"/>
+      <c r="F58" s="44"/>
+      <c r="G58" s="44"/>
+      <c r="H58" s="44"/>
+      <c r="I58" s="44"/>
+      <c r="J58" s="44"/>
+    </row>
+    <row r="59" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A59" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" s="48"/>
+      <c r="C59" s="63">
+        <f>SUMIFS($AI$12:$AI$34, $C$12:$C$34, "Night")</f>
+        <v>0</v>
+      </c>
+      <c r="D59" s="44"/>
+      <c r="E59" s="44"/>
+      <c r="F59" s="44"/>
+      <c r="G59" s="44"/>
+      <c r="H59" s="44"/>
+      <c r="I59" s="44"/>
+      <c r="J59" s="44"/>
+    </row>
+    <row r="60" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A60" s="63"/>
+      <c r="B60" s="47"/>
+      <c r="C60" s="63"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="44"/>
+      <c r="F60" s="44"/>
+      <c r="G60" s="44"/>
+      <c r="H60" s="44"/>
+      <c r="I60" s="44"/>
+      <c r="J60" s="44"/>
+    </row>
+    <row r="61" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A61" s="72" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" s="46"/>
+      <c r="C61" s="63"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="44"/>
+      <c r="G61" s="44"/>
+      <c r="H61" s="44"/>
+      <c r="I61" s="44"/>
+      <c r="J61" s="44"/>
+    </row>
+    <row r="62" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A62" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" s="47"/>
+      <c r="C62" s="63"/>
+      <c r="D62" s="44"/>
+      <c r="E62" s="44"/>
+      <c r="F62" s="44"/>
+      <c r="G62" s="44"/>
+      <c r="H62" s="44"/>
+      <c r="I62" s="44"/>
+      <c r="J62" s="44"/>
+    </row>
+    <row r="63" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A63" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63" s="47"/>
+      <c r="C63" s="63"/>
+      <c r="D63" s="44"/>
+      <c r="E63" s="44"/>
+      <c r="F63" s="44"/>
+      <c r="G63" s="44"/>
+      <c r="H63" s="44"/>
+      <c r="I63" s="44"/>
+      <c r="J63" s="44"/>
+    </row>
+    <row r="64" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A64" s="63"/>
+      <c r="B64" s="47"/>
+      <c r="C64" s="63"/>
+      <c r="D64" s="44"/>
+      <c r="E64" s="44"/>
+      <c r="F64" s="44"/>
+      <c r="G64" s="44"/>
+      <c r="H64" s="44"/>
+      <c r="I64" s="44"/>
+      <c r="J64" s="44"/>
+    </row>
+    <row r="66" ht="155.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="67" ht="169" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="24">
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="E41:J44"/>
     <mergeCell ref="AI9:AI10"/>
     <mergeCell ref="N5:Q5"/>
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="E27:J30"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="AC27:AJ27"/>
-    <mergeCell ref="S28:T32"/>
-    <mergeCell ref="U28:AA32"/>
-    <mergeCell ref="AC28:AJ32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="S33:T37"/>
-    <mergeCell ref="U33:AA37"/>
-    <mergeCell ref="AC33:AJ37"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="S27:AA27"/>
+    <mergeCell ref="A12:A21"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="AC41:AJ41"/>
+    <mergeCell ref="S42:T46"/>
+    <mergeCell ref="U42:AA46"/>
+    <mergeCell ref="AC42:AJ46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="S47:T51"/>
+    <mergeCell ref="U47:AA51"/>
+    <mergeCell ref="AC47:AJ51"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="S41:AA41"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A38:C38"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:B3">
     <cfRule type="expression" dxfId="5" priority="1">
@@ -6361,15 +6984,17 @@
       <formula>TEXT(B3,"mmm")&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9:AH20 D21:AF21 D22:AH25">
-    <cfRule type="expression" dxfId="3" priority="3">
+  <conditionalFormatting sqref="D35:AG35 D36:AH39 D9:AH34">
+    <cfRule type="expression" dxfId="3" priority="34">
+      <formula>D$38=8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36:AH39 D35:AG35 D9:AH34">
+    <cfRule type="expression" dxfId="2" priority="33">
       <formula>OR(D$9="Sat",D$9="Sun")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>D$24=8</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25:AH25">
+  <conditionalFormatting sqref="D39:AH39">
     <cfRule type="cellIs" dxfId="1" priority="5" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
@@ -6393,7 +7018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B05E5B8-DD91-4132-B819-9B05D1BA41C5}">
   <dimension ref="A1:Z67"/>
   <sheetViews>
-    <sheetView zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -6440,7 +7065,7 @@
       <c r="B2" s="5"/>
       <c r="C2" s="94"/>
       <c r="D2" s="99" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="99"/>
@@ -6498,7 +7123,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="94"/>
       <c r="D4" s="100" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="100"/>
@@ -6581,11 +7206,11 @@
     </row>
     <row r="7" spans="1:26" ht="26.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C7" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D7" s="36"/>
       <c r="E7" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="12"/>
@@ -6594,7 +7219,7 @@
       <c r="C8" s="10"/>
       <c r="D8" s="37"/>
       <c r="E8" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="12"/>
@@ -6608,27 +7233,27 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B10" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="95" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="95" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="95" t="s">
+      <c r="E10" s="101" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="95" t="s">
+      <c r="F10" s="95" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="101" t="s">
+      <c r="G10" s="13" t="s">
         <v>80</v>
-      </c>
-      <c r="F10" s="95" t="s">
-        <v>81</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="38" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C11" s="96"/>
       <c r="D11" s="96"/>
@@ -6644,16 +7269,16 @@
         <v>0</v>
       </c>
       <c r="D12" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="G12" s="17" t="s">
         <v>85</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="26" x14ac:dyDescent="0.35">
@@ -6664,16 +7289,16 @@
         <v>6</v>
       </c>
       <c r="D13" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="19" t="s">
         <v>88</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>90</v>
       </c>
       <c r="H13" s="3"/>
     </row>
@@ -6682,19 +7307,19 @@
         <v>3</v>
       </c>
       <c r="C14" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="G14" s="19" t="s">
         <v>92</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>94</v>
       </c>
       <c r="H14" s="23"/>
     </row>
@@ -6706,16 +7331,16 @@
         <v>18</v>
       </c>
       <c r="D15" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15" s="19" t="s">
         <v>95</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>97</v>
       </c>
       <c r="H15" s="23"/>
     </row>
@@ -6727,16 +7352,16 @@
         <v>8</v>
       </c>
       <c r="D16" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" s="19" t="s">
         <v>98</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>100</v>
       </c>
       <c r="H16" s="23"/>
     </row>
@@ -6748,16 +7373,16 @@
         <v>14</v>
       </c>
       <c r="D17" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" s="19" t="s">
         <v>101</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>103</v>
       </c>
       <c r="H17" s="23"/>
     </row>
@@ -6766,19 +7391,19 @@
         <v>7</v>
       </c>
       <c r="C18" s="138" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="G18" s="19" t="s">
         <v>105</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="G18" s="19" t="s">
-        <v>107</v>
       </c>
       <c r="H18" s="23"/>
     </row>
@@ -6787,25 +7412,25 @@
         <v>8</v>
       </c>
       <c r="C19" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="G19" s="21" t="s">
         <v>109</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>111</v>
       </c>
       <c r="H19" s="24"/>
     </row>
     <row r="20" spans="2:8" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C20" s="96"/>
       <c r="D20" s="96"/>
@@ -6819,19 +7444,19 @@
         <v>9</v>
       </c>
       <c r="C21" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="G21" s="19" t="s">
         <v>114</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>116</v>
       </c>
       <c r="H21" s="24"/>
     </row>
@@ -6843,16 +7468,16 @@
         <v>21</v>
       </c>
       <c r="D22" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="G22" s="25" t="s">
         <v>117</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="G22" s="25" t="s">
-        <v>119</v>
       </c>
       <c r="H22" s="24"/>
     </row>
@@ -6861,19 +7486,19 @@
         <v>11</v>
       </c>
       <c r="C23" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="G23" s="19" t="s">
         <v>121</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="G23" s="19" t="s">
-        <v>123</v>
       </c>
       <c r="H23" s="1"/>
     </row>
@@ -6882,19 +7507,19 @@
         <v>12</v>
       </c>
       <c r="C24" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="F24" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="G24" s="19" t="s">
         <v>126</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="G24" s="19" t="s">
-        <v>128</v>
       </c>
       <c r="H24" s="24"/>
     </row>
@@ -6903,19 +7528,19 @@
         <v>13</v>
       </c>
       <c r="C25" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F25" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="G25" s="19" t="s">
         <v>130</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>132</v>
       </c>
       <c r="H25" s="1"/>
     </row>
@@ -6924,23 +7549,23 @@
         <v>14</v>
       </c>
       <c r="C26" s="103" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F26" s="27"/>
       <c r="G26" s="30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="2:8" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="104" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C27" s="105"/>
       <c r="D27" s="105"/>
@@ -6957,10 +7582,10 @@
         <v>52</v>
       </c>
       <c r="D28" s="109" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F28" s="110"/>
       <c r="G28" s="111"/>
@@ -6974,10 +7599,10 @@
         <v>56</v>
       </c>
       <c r="D29" s="109" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F29" s="113"/>
       <c r="G29" s="114"/>
@@ -6991,10 +7616,10 @@
         <v>57</v>
       </c>
       <c r="D30" s="109" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F30" s="113"/>
       <c r="G30" s="114"/>
@@ -7008,10 +7633,10 @@
         <v>58</v>
       </c>
       <c r="D31" s="109" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F31" s="113"/>
       <c r="G31" s="114"/>
@@ -7025,10 +7650,10 @@
         <v>59</v>
       </c>
       <c r="D32" s="109" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F32" s="113"/>
       <c r="G32" s="114"/>
@@ -7042,10 +7667,10 @@
         <v>60</v>
       </c>
       <c r="D33" s="109" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F33" s="113"/>
       <c r="G33" s="114"/>
@@ -7059,10 +7684,10 @@
         <v>62</v>
       </c>
       <c r="D34" s="109" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F34" s="113"/>
       <c r="G34" s="114"/>
@@ -7073,19 +7698,19 @@
         <v>22</v>
       </c>
       <c r="C35" s="116" t="s">
+        <v>143</v>
+      </c>
+      <c r="D35" s="117" t="s">
+        <v>144</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="F35" s="118" t="s">
         <v>145</v>
       </c>
-      <c r="D35" s="117" t="s">
+      <c r="G35" s="119" t="s">
         <v>146</v>
-      </c>
-      <c r="E35" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="F35" s="118" t="s">
-        <v>147</v>
-      </c>
-      <c r="G35" s="119" t="s">
-        <v>148</v>
       </c>
       <c r="H35" s="24"/>
     </row>
@@ -7097,10 +7722,10 @@
         <v>64</v>
       </c>
       <c r="D36" s="121" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F36" s="113"/>
       <c r="G36" s="114"/>
@@ -7114,10 +7739,10 @@
         <v>65</v>
       </c>
       <c r="D37" s="121" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F37" s="113"/>
       <c r="G37" s="114"/>
@@ -7131,10 +7756,10 @@
         <v>66</v>
       </c>
       <c r="D38" s="121" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F38" s="113"/>
       <c r="G38" s="114"/>
@@ -7145,17 +7770,17 @@
         <v>26</v>
       </c>
       <c r="C39" s="115" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D39" s="122" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E39" s="122" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F39" s="121"/>
       <c r="G39" s="121" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H39" s="24"/>
     </row>
@@ -7164,19 +7789,19 @@
         <v>27</v>
       </c>
       <c r="C40" s="115" t="s">
+        <v>153</v>
+      </c>
+      <c r="D40" s="122" t="s">
+        <v>154</v>
+      </c>
+      <c r="E40" s="119" t="s">
         <v>155</v>
       </c>
-      <c r="D40" s="122" t="s">
+      <c r="F40" s="122" t="s">
         <v>156</v>
       </c>
-      <c r="E40" s="119" t="s">
+      <c r="G40" s="119" t="s">
         <v>157</v>
-      </c>
-      <c r="F40" s="122" t="s">
-        <v>158</v>
-      </c>
-      <c r="G40" s="119" t="s">
-        <v>159</v>
       </c>
       <c r="H40" s="24"/>
     </row>
@@ -7185,19 +7810,19 @@
         <v>28</v>
       </c>
       <c r="C41" s="115" t="s">
+        <v>158</v>
+      </c>
+      <c r="D41" s="122" t="s">
+        <v>159</v>
+      </c>
+      <c r="E41" s="119" t="s">
         <v>160</v>
       </c>
-      <c r="D41" s="122" t="s">
+      <c r="F41" s="122" t="s">
         <v>161</v>
       </c>
-      <c r="E41" s="119" t="s">
+      <c r="G41" s="119" t="s">
         <v>162</v>
-      </c>
-      <c r="F41" s="122" t="s">
-        <v>163</v>
-      </c>
-      <c r="G41" s="119" t="s">
-        <v>164</v>
       </c>
       <c r="H41" s="24"/>
     </row>
@@ -7247,7 +7872,7 @@
       <c r="C47" s="129"/>
       <c r="D47" s="122"/>
       <c r="E47" s="119"/>
-      <c r="F47" s="199"/>
+      <c r="F47" s="204"/>
       <c r="G47" s="122"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.35">
@@ -7255,7 +7880,7 @@
       <c r="C48" s="128"/>
       <c r="D48" s="122"/>
       <c r="E48" s="119"/>
-      <c r="F48" s="199"/>
+      <c r="F48" s="204"/>
       <c r="G48" s="122"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.35">
@@ -7263,7 +7888,7 @@
       <c r="C49" s="128"/>
       <c r="D49" s="122"/>
       <c r="E49" s="119"/>
-      <c r="F49" s="199"/>
+      <c r="F49" s="204"/>
       <c r="G49" s="122"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.35">
@@ -7271,7 +7896,7 @@
       <c r="C50" s="129"/>
       <c r="D50" s="122"/>
       <c r="E50" s="119"/>
-      <c r="F50" s="199"/>
+      <c r="F50" s="204"/>
       <c r="G50" s="122"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.35">

</xml_diff>